<commit_message>
adding Saarland 2022 election and Rehlinger Cabinet
</commit_message>
<xml_diff>
--- a/inst/extdata/additional_elecdata.xlsx
+++ b/inst/extdata/additional_elecdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Git_Projekte\bundeslaendeR\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertstelzle/Documents/addingsaarland/bundeslaendeR/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33564F78-EC63-4189-BD71-CB85B1271B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B84CACF-701F-044B-851C-7318307BD2B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="154">
   <si>
     <t>state</t>
   </si>
@@ -460,16 +460,59 @@
   </si>
   <si>
     <t>2021-06-06</t>
+  </si>
+  <si>
+    <t>SL</t>
+  </si>
+  <si>
+    <t>2022-03-27</t>
+  </si>
+  <si>
+    <t>Familie</t>
+  </si>
+  <si>
+    <t>FAMILIE</t>
+  </si>
+  <si>
+    <t>Familien-Partei Deutschlands</t>
+  </si>
+  <si>
+    <t>FW-SL</t>
+  </si>
+  <si>
+    <t>bunt.saar</t>
+  </si>
+  <si>
+    <t>bunt.saar sozial-ökologische liste</t>
+  </si>
+  <si>
+    <t>Okologisch-Demokratische Partei</t>
+  </si>
+  <si>
+    <t>Partei für Arbeit, Rechtsstaat, Tierschutz, Elitenförderungu und basisdemokratische Initiative</t>
+  </si>
+  <si>
+    <t>SGV</t>
+  </si>
+  <si>
+    <t>SGV Solidarität, Gerechtigkeit, Veränderung</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -495,10 +538,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -779,30 +823,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L86"/>
+  <dimension ref="A1:L104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.85546875" customWidth="1"/>
-    <col min="11" max="11" width="90.7109375" customWidth="1"/>
-    <col min="12" max="12" width="16.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.83203125" customWidth="1"/>
+    <col min="11" max="11" width="90.6640625" customWidth="1"/>
+    <col min="12" max="12" width="16.83203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -840,7 +884,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -878,7 +922,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -916,7 +960,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -954,7 +998,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -992,7 +1036,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1030,7 +1074,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1068,7 +1112,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1106,7 +1150,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1144,7 +1188,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1182,7 +1226,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1220,7 +1264,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1258,7 +1302,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -1296,7 +1340,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -1334,7 +1378,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -1372,7 +1416,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
@@ -1410,7 +1454,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
@@ -1448,7 +1492,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
@@ -1486,7 +1530,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
@@ -1524,7 +1568,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
@@ -1562,7 +1606,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
@@ -1600,7 +1644,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
@@ -1638,7 +1682,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>10</v>
       </c>
@@ -1676,7 +1720,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>10</v>
       </c>
@@ -1714,7 +1758,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
@@ -1752,7 +1796,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>34</v>
       </c>
@@ -1790,7 +1834,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>34</v>
       </c>
@@ -1828,7 +1872,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
@@ -1866,7 +1910,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>34</v>
       </c>
@@ -1904,7 +1948,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>34</v>
       </c>
@@ -1942,7 +1986,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>34</v>
       </c>
@@ -1980,7 +2024,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
@@ -2018,7 +2062,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>34</v>
       </c>
@@ -2056,7 +2100,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>34</v>
       </c>
@@ -2094,7 +2138,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -2132,7 +2176,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
@@ -2170,7 +2214,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>34</v>
       </c>
@@ -2208,7 +2252,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>34</v>
       </c>
@@ -2246,7 +2290,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>34</v>
       </c>
@@ -2284,7 +2328,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>34</v>
       </c>
@@ -2322,7 +2366,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>34</v>
       </c>
@@ -2360,7 +2404,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>34</v>
       </c>
@@ -2398,7 +2442,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>34</v>
       </c>
@@ -2436,7 +2480,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>34</v>
       </c>
@@ -2474,7 +2518,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>34</v>
       </c>
@@ -2512,7 +2556,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>34</v>
       </c>
@@ -2550,7 +2594,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>34</v>
       </c>
@@ -2588,7 +2632,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>34</v>
       </c>
@@ -2626,7 +2670,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>34</v>
       </c>
@@ -2664,7 +2708,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>34</v>
       </c>
@@ -2702,7 +2746,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>34</v>
       </c>
@@ -2740,7 +2784,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>34</v>
       </c>
@@ -2778,7 +2822,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>34</v>
       </c>
@@ -2816,7 +2860,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>34</v>
       </c>
@@ -2854,7 +2898,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>34</v>
       </c>
@@ -2892,7 +2936,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>34</v>
       </c>
@@ -2930,7 +2974,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>34</v>
       </c>
@@ -2968,7 +3012,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>34</v>
       </c>
@@ -3006,7 +3050,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>34</v>
       </c>
@@ -3044,7 +3088,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>34</v>
       </c>
@@ -3082,7 +3126,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>34</v>
       </c>
@@ -3120,7 +3164,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>34</v>
       </c>
@@ -3158,7 +3202,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>122</v>
       </c>
@@ -3196,7 +3240,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>122</v>
       </c>
@@ -3234,7 +3278,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>122</v>
       </c>
@@ -3272,7 +3316,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>122</v>
       </c>
@@ -3310,7 +3354,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>122</v>
       </c>
@@ -3348,7 +3392,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>122</v>
       </c>
@@ -3386,7 +3430,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>122</v>
       </c>
@@ -3424,7 +3468,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>122</v>
       </c>
@@ -3462,7 +3506,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>122</v>
       </c>
@@ -3500,7 +3544,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>122</v>
       </c>
@@ -3532,13 +3576,13 @@
         <v>41</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>54</v>
+        <v>151</v>
       </c>
       <c r="L72" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>122</v>
       </c>
@@ -3576,7 +3620,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>122</v>
       </c>
@@ -3614,7 +3658,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>122</v>
       </c>
@@ -3652,7 +3696,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>122</v>
       </c>
@@ -3690,7 +3734,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>122</v>
       </c>
@@ -3728,7 +3772,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>122</v>
       </c>
@@ -3766,7 +3810,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>122</v>
       </c>
@@ -3804,7 +3848,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>122</v>
       </c>
@@ -3842,7 +3886,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>122</v>
       </c>
@@ -3880,7 +3924,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>122</v>
       </c>
@@ -3918,7 +3962,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>122</v>
       </c>
@@ -3956,7 +4000,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>122</v>
       </c>
@@ -3994,7 +4038,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>122</v>
       </c>
@@ -4032,7 +4076,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>122</v>
       </c>
@@ -4068,6 +4112,690 @@
       </c>
       <c r="L86" s="2" t="s">
         <v>140</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B87" s="1">
+        <v>17</v>
+      </c>
+      <c r="C87" s="1">
+        <v>746307</v>
+      </c>
+      <c r="D87" s="1">
+        <v>458113</v>
+      </c>
+      <c r="E87" s="1">
+        <v>452411</v>
+      </c>
+      <c r="F87" s="1">
+        <v>51</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H87" s="1">
+        <v>129154</v>
+      </c>
+      <c r="I87" s="1">
+        <v>19</v>
+      </c>
+      <c r="J87" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K87" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L87" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B88" s="1">
+        <v>17</v>
+      </c>
+      <c r="C88" s="1">
+        <v>746307</v>
+      </c>
+      <c r="D88" s="1">
+        <v>458113</v>
+      </c>
+      <c r="E88" s="1">
+        <v>452411</v>
+      </c>
+      <c r="F88" s="1">
+        <v>51</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H88" s="1">
+        <v>196801</v>
+      </c>
+      <c r="I88">
+        <v>29</v>
+      </c>
+      <c r="J88" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K88" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L88" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B89" s="1">
+        <v>17</v>
+      </c>
+      <c r="C89" s="1">
+        <v>746307</v>
+      </c>
+      <c r="D89" s="1">
+        <v>458113</v>
+      </c>
+      <c r="E89" s="1">
+        <v>452411</v>
+      </c>
+      <c r="F89" s="1">
+        <v>51</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H89" s="1">
+        <v>11689</v>
+      </c>
+      <c r="I89">
+        <v>0</v>
+      </c>
+      <c r="J89" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K89" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L89" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B90" s="1">
+        <v>17</v>
+      </c>
+      <c r="C90" s="1">
+        <v>746307</v>
+      </c>
+      <c r="D90" s="1">
+        <v>458113</v>
+      </c>
+      <c r="E90" s="1">
+        <v>452411</v>
+      </c>
+      <c r="F90" s="1">
+        <v>51</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H90" s="1">
+        <v>25719</v>
+      </c>
+      <c r="I90">
+        <v>3</v>
+      </c>
+      <c r="J90" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K90" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L90" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B91" s="1">
+        <v>17</v>
+      </c>
+      <c r="C91" s="1">
+        <v>746307</v>
+      </c>
+      <c r="D91" s="1">
+        <v>458113</v>
+      </c>
+      <c r="E91" s="1">
+        <v>452411</v>
+      </c>
+      <c r="F91" s="1">
+        <v>51</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H91" s="1">
+        <v>22598</v>
+      </c>
+      <c r="I91">
+        <v>0</v>
+      </c>
+      <c r="J91" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K91" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L91" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B92" s="1">
+        <v>17</v>
+      </c>
+      <c r="C92" s="1">
+        <v>746307</v>
+      </c>
+      <c r="D92" s="1">
+        <v>458113</v>
+      </c>
+      <c r="E92" s="1">
+        <v>452411</v>
+      </c>
+      <c r="F92" s="1">
+        <v>51</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H92" s="1">
+        <v>21618</v>
+      </c>
+      <c r="I92">
+        <v>0</v>
+      </c>
+      <c r="J92" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K92" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L92" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B93" s="1">
+        <v>17</v>
+      </c>
+      <c r="C93" s="1">
+        <v>746307</v>
+      </c>
+      <c r="D93" s="1">
+        <v>458113</v>
+      </c>
+      <c r="E93" s="1">
+        <v>452411</v>
+      </c>
+      <c r="F93" s="1">
+        <v>51</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H93" s="1">
+        <v>3836</v>
+      </c>
+      <c r="I93">
+        <v>0</v>
+      </c>
+      <c r="J93" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="K93" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="L93" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B94" s="1">
+        <v>17</v>
+      </c>
+      <c r="C94" s="1">
+        <v>746307</v>
+      </c>
+      <c r="D94" s="1">
+        <v>458113</v>
+      </c>
+      <c r="E94" s="1">
+        <v>452411</v>
+      </c>
+      <c r="F94" s="1">
+        <v>51</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H94" s="1">
+        <v>1318</v>
+      </c>
+      <c r="I94">
+        <v>0</v>
+      </c>
+      <c r="J94" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K94" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L94" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B95" s="1">
+        <v>17</v>
+      </c>
+      <c r="C95" s="1">
+        <v>746307</v>
+      </c>
+      <c r="D95" s="1">
+        <v>458113</v>
+      </c>
+      <c r="E95" s="1">
+        <v>452411</v>
+      </c>
+      <c r="F95" s="1">
+        <v>51</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H95" s="1">
+        <v>7636</v>
+      </c>
+      <c r="I95">
+        <v>0</v>
+      </c>
+      <c r="J95" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K95" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L95" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B96" s="1">
+        <v>17</v>
+      </c>
+      <c r="C96" s="1">
+        <v>746307</v>
+      </c>
+      <c r="D96" s="1">
+        <v>458113</v>
+      </c>
+      <c r="E96" s="1">
+        <v>452411</v>
+      </c>
+      <c r="F96" s="1">
+        <v>51</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H96" s="1">
+        <v>6448</v>
+      </c>
+      <c r="I96">
+        <v>0</v>
+      </c>
+      <c r="J96" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K96" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L96" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B97" s="1">
+        <v>17</v>
+      </c>
+      <c r="C97" s="1">
+        <v>746307</v>
+      </c>
+      <c r="D97" s="1">
+        <v>458113</v>
+      </c>
+      <c r="E97" s="1">
+        <v>452411</v>
+      </c>
+      <c r="F97" s="1">
+        <v>51</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H97" s="1">
+        <v>6216</v>
+      </c>
+      <c r="I97">
+        <v>0</v>
+      </c>
+      <c r="J97" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K97" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="L97" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B98" s="1">
+        <v>17</v>
+      </c>
+      <c r="C98" s="1">
+        <v>746307</v>
+      </c>
+      <c r="D98" s="1">
+        <v>458113</v>
+      </c>
+      <c r="E98" s="1">
+        <v>452411</v>
+      </c>
+      <c r="F98" s="1">
+        <v>51</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H98" s="1">
+        <v>613</v>
+      </c>
+      <c r="I98">
+        <v>0</v>
+      </c>
+      <c r="J98" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K98" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="L98" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B99" s="1">
+        <v>17</v>
+      </c>
+      <c r="C99" s="1">
+        <v>746307</v>
+      </c>
+      <c r="D99" s="1">
+        <v>458113</v>
+      </c>
+      <c r="E99" s="1">
+        <v>452411</v>
+      </c>
+      <c r="F99" s="1">
+        <v>51</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H99" s="1">
+        <v>233</v>
+      </c>
+      <c r="I99">
+        <v>0</v>
+      </c>
+      <c r="J99" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K99" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L99" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B100" s="1">
+        <v>17</v>
+      </c>
+      <c r="C100" s="1">
+        <v>746307</v>
+      </c>
+      <c r="D100" s="1">
+        <v>458113</v>
+      </c>
+      <c r="E100" s="1">
+        <v>452411</v>
+      </c>
+      <c r="F100" s="1">
+        <v>51</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H100" s="1">
+        <v>4716</v>
+      </c>
+      <c r="I100">
+        <v>0</v>
+      </c>
+      <c r="J100" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K100" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="L100" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B101" s="1">
+        <v>17</v>
+      </c>
+      <c r="C101" s="1">
+        <v>746307</v>
+      </c>
+      <c r="D101" s="1">
+        <v>458113</v>
+      </c>
+      <c r="E101" s="1">
+        <v>452411</v>
+      </c>
+      <c r="F101" s="1">
+        <v>51</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H101" s="1">
+        <v>368</v>
+      </c>
+      <c r="I101">
+        <v>0</v>
+      </c>
+      <c r="J101" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K101" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L101" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A102" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B102" s="1">
+        <v>17</v>
+      </c>
+      <c r="C102" s="1">
+        <v>746307</v>
+      </c>
+      <c r="D102" s="1">
+        <v>458113</v>
+      </c>
+      <c r="E102" s="1">
+        <v>452411</v>
+      </c>
+      <c r="F102" s="1">
+        <v>51</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H102" s="1">
+        <v>10391</v>
+      </c>
+      <c r="I102">
+        <v>0</v>
+      </c>
+      <c r="J102" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K102" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L102" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B103" s="1">
+        <v>17</v>
+      </c>
+      <c r="C103" s="1">
+        <v>746307</v>
+      </c>
+      <c r="D103" s="1">
+        <v>458113</v>
+      </c>
+      <c r="E103" s="1">
+        <v>452411</v>
+      </c>
+      <c r="F103" s="1">
+        <v>51</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H103" s="1">
+        <v>412</v>
+      </c>
+      <c r="I103">
+        <v>0</v>
+      </c>
+      <c r="J103" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="K103" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="L103" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A104" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B104" s="1">
+        <v>17</v>
+      </c>
+      <c r="C104" s="1">
+        <v>746307</v>
+      </c>
+      <c r="D104" s="1">
+        <v>458113</v>
+      </c>
+      <c r="E104" s="1">
+        <v>452411</v>
+      </c>
+      <c r="F104" s="1">
+        <v>51</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H104" s="1">
+        <v>2645</v>
+      </c>
+      <c r="I104">
+        <v>0</v>
+      </c>
+      <c r="J104" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K104" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L104" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add nds22 election and weil III gov. and fix weils name which for whatever reason i had wrong
</commit_message>
<xml_diff>
--- a/inst/extdata/additional_elecdata.xlsx
+++ b/inst/extdata/additional_elecdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\bldrt\bundeslaendeR\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertstelzle/git_projekte/add_nds21/bundeslaendeR/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5DC6182-68B0-46B4-B378-F22528015AEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31040369-54F7-9343-8CDB-C323120F3D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="18000" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="192">
   <si>
     <t>state</t>
   </si>
@@ -195,9 +195,6 @@
     <t>PARTEI MENSCH UMWELT TIERSCHUTZ</t>
   </si>
   <si>
-    <t>Partei für Arbeit, Rechtsstaat, Tierschutz, Elitenförderungu nd basisdemokratische Initiative</t>
-  </si>
-  <si>
     <t>Aktion Partei für Tierschutz – TIERSCHUTZ hier!</t>
   </si>
   <si>
@@ -574,13 +571,52 @@
   </si>
   <si>
     <t>Z.</t>
+  </si>
+  <si>
+    <t>NI</t>
+  </si>
+  <si>
+    <t>DIE LINKE.</t>
+  </si>
+  <si>
+    <t>Die Humanisten Niedersachsen</t>
+  </si>
+  <si>
+    <t>Christlich Demokratische Union Deutschlands in Niedersachsen</t>
+  </si>
+  <si>
+    <t>DIE LINKE. Niedersachsen</t>
+  </si>
+  <si>
+    <t>Basisdemokratische Partei Deutschland Landesverband Niedersachsen</t>
+  </si>
+  <si>
+    <t>FREIE WÄHLER Niedersachsen</t>
+  </si>
+  <si>
+    <t>Partei der Humanisten Niedersachsen</t>
+  </si>
+  <si>
+    <t>PARTEI MENSCH UMWELT TIERSCHUTZ Landesverband Niedersachsen</t>
+  </si>
+  <si>
+    <t>Piratenpartei Niedersachsen</t>
+  </si>
+  <si>
+    <t>Volt Deutschland Landesverband Niedersachsen</t>
+  </si>
+  <si>
+    <t>FW-NI</t>
+  </si>
+  <si>
+    <t>2022-10-09</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -594,6 +630,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -616,7 +658,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -624,6 +666,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -904,30 +947,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L144"/>
+  <dimension ref="A1:L167"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K124" sqref="K124"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G159" sqref="G159"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.85546875" customWidth="1"/>
-    <col min="11" max="11" width="90.7109375" customWidth="1"/>
-    <col min="12" max="12" width="16.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.83203125" customWidth="1"/>
+    <col min="11" max="11" width="90.6640625" customWidth="1"/>
+    <col min="12" max="12" width="16.83203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -962,10 +1005,10 @@
         <v>34</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1000,10 +1043,10 @@
         <v>46</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1038,10 +1081,10 @@
         <v>47</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1076,10 +1119,10 @@
         <v>35</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1114,10 +1157,10 @@
         <v>48</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1152,10 +1195,10 @@
         <v>49</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1190,10 +1233,10 @@
         <v>50</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1228,10 +1271,10 @@
         <v>37</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1266,10 +1309,10 @@
         <v>51</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1304,10 +1347,10 @@
         <v>52</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1342,10 +1385,10 @@
         <v>39</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1377,13 +1420,13 @@
         <v>40</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -1415,13 +1458,13 @@
         <v>41</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -1453,13 +1496,13 @@
         <v>23</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -1491,13 +1534,13 @@
         <v>42</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
@@ -1529,13 +1572,13 @@
         <v>43</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
@@ -1567,13 +1610,13 @@
         <v>26</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
@@ -1608,10 +1651,10 @@
         <v>44</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
@@ -1643,13 +1686,13 @@
         <v>28</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
@@ -1681,13 +1724,13 @@
         <v>29</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
@@ -1719,13 +1762,13 @@
         <v>30</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
@@ -1757,13 +1800,13 @@
         <v>45</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>10</v>
       </c>
@@ -1795,13 +1838,13 @@
         <v>32</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>33</v>
       </c>
@@ -1836,10 +1879,10 @@
         <v>48</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
@@ -1874,10 +1917,10 @@
         <v>46</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>33</v>
       </c>
@@ -1912,10 +1955,10 @@
         <v>50</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
@@ -1950,10 +1993,10 @@
         <v>35</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
@@ -1988,10 +2031,10 @@
         <v>47</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>33</v>
       </c>
@@ -2026,10 +2069,10 @@
         <v>49</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
@@ -2061,13 +2104,13 @@
         <v>40</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>53</v>
+        <v>140</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
@@ -2102,10 +2145,10 @@
         <v>52</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>33</v>
       </c>
@@ -2137,13 +2180,13 @@
         <v>43</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
@@ -2163,7 +2206,7 @@
         <v>147</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H33" s="1">
         <v>8910</v>
@@ -2172,16 +2215,16 @@
         <v>0</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
@@ -2213,13 +2256,13 @@
         <v>26</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
@@ -2251,13 +2294,13 @@
         <v>24</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
@@ -2289,13 +2332,13 @@
         <v>32</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>33</v>
       </c>
@@ -2315,7 +2358,7 @@
         <v>147</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H37" s="1">
         <v>2359</v>
@@ -2324,16 +2367,16 @@
         <v>0</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>33</v>
       </c>
@@ -2353,7 +2396,7 @@
         <v>147</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H38" s="1">
         <v>492</v>
@@ -2362,16 +2405,16 @@
         <v>0</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>33</v>
       </c>
@@ -2391,7 +2434,7 @@
         <v>147</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H39" s="1">
         <v>575</v>
@@ -2400,16 +2443,16 @@
         <v>0</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>33</v>
       </c>
@@ -2429,7 +2472,7 @@
         <v>147</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H40" s="1">
         <v>174</v>
@@ -2438,16 +2481,16 @@
         <v>0</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>33</v>
       </c>
@@ -2467,7 +2510,7 @@
         <v>147</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H41" s="1">
         <v>1713</v>
@@ -2476,16 +2519,16 @@
         <v>0</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>33</v>
       </c>
@@ -2517,13 +2560,13 @@
         <v>30</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>33</v>
       </c>
@@ -2555,13 +2598,13 @@
         <v>41</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>33</v>
       </c>
@@ -2596,10 +2639,10 @@
         <v>51</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>33</v>
       </c>
@@ -2619,7 +2662,7 @@
         <v>147</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H45" s="1">
         <v>2486</v>
@@ -2628,16 +2671,16 @@
         <v>0</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>33</v>
       </c>
@@ -2657,7 +2700,7 @@
         <v>147</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H46" s="1">
         <v>9</v>
@@ -2666,16 +2709,16 @@
         <v>0</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>33</v>
       </c>
@@ -2695,7 +2738,7 @@
         <v>147</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H47" s="1">
         <v>12654</v>
@@ -2704,16 +2747,16 @@
         <v>0</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>33</v>
       </c>
@@ -2733,7 +2776,7 @@
         <v>147</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H48" s="1">
         <v>95</v>
@@ -2742,16 +2785,16 @@
         <v>0</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>33</v>
       </c>
@@ -2771,7 +2814,7 @@
         <v>147</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H49" s="1">
         <v>55</v>
@@ -2780,16 +2823,16 @@
         <v>0</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>33</v>
       </c>
@@ -2809,7 +2852,7 @@
         <v>147</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H50" s="1">
         <v>3587</v>
@@ -2818,16 +2861,16 @@
         <v>0</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>33</v>
       </c>
@@ -2847,7 +2890,7 @@
         <v>147</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H51" s="1">
         <v>970</v>
@@ -2856,16 +2899,16 @@
         <v>0</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>33</v>
       </c>
@@ -2885,7 +2928,7 @@
         <v>147</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H52" s="1">
         <v>15297</v>
@@ -2900,10 +2943,10 @@
         <v>37</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>33</v>
       </c>
@@ -2932,16 +2975,16 @@
         <v>0</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>33</v>
       </c>
@@ -2961,7 +3004,7 @@
         <v>147</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H54" s="1">
         <v>4261</v>
@@ -2970,16 +3013,16 @@
         <v>0</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>33</v>
       </c>
@@ -3011,13 +3054,13 @@
         <v>29</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>33</v>
       </c>
@@ -3037,7 +3080,7 @@
         <v>147</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H56" s="1">
         <v>18853</v>
@@ -3046,16 +3089,16 @@
         <v>0</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>33</v>
       </c>
@@ -3075,7 +3118,7 @@
         <v>147</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H57" s="1">
         <v>20205</v>
@@ -3084,18 +3127,18 @@
         <v>0</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K57" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="L57" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="L57" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="B58" s="1">
         <v>8</v>
@@ -3128,12 +3171,12 @@
         <v>48</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B59" s="1">
         <v>8</v>
@@ -3166,12 +3209,12 @@
         <v>47</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B60" s="1">
         <v>8</v>
@@ -3204,12 +3247,12 @@
         <v>46</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B61" s="1">
         <v>8</v>
@@ -3242,12 +3285,12 @@
         <v>35</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B62" s="1">
         <v>8</v>
@@ -3280,12 +3323,12 @@
         <v>50</v>
       </c>
       <c r="L62" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B63" s="1">
         <v>8</v>
@@ -3318,12 +3361,12 @@
         <v>49</v>
       </c>
       <c r="L63" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B64" s="1">
         <v>8</v>
@@ -3353,15 +3396,15 @@
         <v>26</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L64" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B65" s="1">
         <v>8</v>
@@ -3394,12 +3437,12 @@
         <v>52</v>
       </c>
       <c r="L65" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B66" s="1">
         <v>8</v>
@@ -3417,7 +3460,7 @@
         <v>79</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H66" s="1">
         <v>3348</v>
@@ -3426,18 +3469,18 @@
         <v>0</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L66" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B67" s="1">
         <v>8</v>
@@ -3467,15 +3510,15 @@
         <v>40</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L67" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B68" s="1">
         <v>8</v>
@@ -3493,7 +3536,7 @@
         <v>79</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H68" s="1">
         <v>10075</v>
@@ -3505,15 +3548,15 @@
         <v>37</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L68" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B69" s="1">
         <v>8</v>
@@ -3543,15 +3586,15 @@
         <v>43</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L69" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B70" s="1">
         <v>8</v>
@@ -3569,7 +3612,7 @@
         <v>79</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H70" s="1">
         <v>727</v>
@@ -3578,18 +3621,18 @@
         <v>0</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L70" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B71" s="1">
         <v>8</v>
@@ -3607,7 +3650,7 @@
         <v>79</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H71" s="1">
         <v>827</v>
@@ -3616,18 +3659,18 @@
         <v>0</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L71" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B72" s="1">
         <v>8</v>
@@ -3657,15 +3700,15 @@
         <v>41</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L72" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B73" s="1">
         <v>8</v>
@@ -3695,15 +3738,15 @@
         <v>18</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L73" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B74" s="1">
         <v>8</v>
@@ -3721,7 +3764,7 @@
         <v>79</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H74" s="1">
         <v>563</v>
@@ -3730,18 +3773,18 @@
         <v>0</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L74" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B75" s="1">
         <v>8</v>
@@ -3759,7 +3802,7 @@
         <v>79</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H75" s="1">
         <v>436</v>
@@ -3768,18 +3811,18 @@
         <v>0</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K75" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L75" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B76" s="1">
         <v>8</v>
@@ -3809,15 +3852,15 @@
         <v>32</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L76" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B77" s="1">
         <v>8</v>
@@ -3847,15 +3890,15 @@
         <v>30</v>
       </c>
       <c r="K77" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L77" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B78" s="1">
         <v>8</v>
@@ -3885,15 +3928,15 @@
         <v>29</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L78" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B79" s="1">
         <v>8</v>
@@ -3923,15 +3966,15 @@
         <v>24</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L79" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B80" s="1">
         <v>8</v>
@@ -3949,7 +3992,7 @@
         <v>79</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H80" s="1">
         <v>1631</v>
@@ -3958,18 +4001,18 @@
         <v>0</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L80" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B81" s="1">
         <v>8</v>
@@ -3987,7 +4030,7 @@
         <v>79</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H81" s="1">
         <v>2331</v>
@@ -3996,18 +4039,18 @@
         <v>0</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K81" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L81" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B82" s="1">
         <v>17</v>
@@ -4040,12 +4083,12 @@
         <v>46</v>
       </c>
       <c r="L82" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B83" s="1">
         <v>17</v>
@@ -4078,12 +4121,12 @@
         <v>48</v>
       </c>
       <c r="L83" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B84" s="1">
         <v>17</v>
@@ -4116,12 +4159,12 @@
         <v>35</v>
       </c>
       <c r="L84" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B85" s="1">
         <v>17</v>
@@ -4154,12 +4197,12 @@
         <v>47</v>
       </c>
       <c r="L85" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B86" s="1">
         <v>17</v>
@@ -4192,12 +4235,12 @@
         <v>50</v>
       </c>
       <c r="L86" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B87" s="1">
         <v>17</v>
@@ -4230,12 +4273,12 @@
         <v>49</v>
       </c>
       <c r="L87" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B88" s="1">
         <v>17</v>
@@ -4253,7 +4296,7 @@
         <v>51</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H88" s="1">
         <v>3836</v>
@@ -4262,18 +4305,18 @@
         <v>0</v>
       </c>
       <c r="J88" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="K88" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="K88" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="L88" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B89" s="1">
         <v>17</v>
@@ -4303,15 +4346,15 @@
         <v>43</v>
       </c>
       <c r="K89" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L89" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B90" s="1">
         <v>17</v>
@@ -4329,7 +4372,7 @@
         <v>51</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H90" s="1">
         <v>7636</v>
@@ -4344,12 +4387,12 @@
         <v>37</v>
       </c>
       <c r="L90" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B91" s="1">
         <v>17</v>
@@ -4382,12 +4425,12 @@
         <v>51</v>
       </c>
       <c r="L91" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B92" s="1">
         <v>17</v>
@@ -4405,7 +4448,7 @@
         <v>51</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H92" s="1">
         <v>6216</v>
@@ -4414,18 +4457,18 @@
         <v>0</v>
       </c>
       <c r="J92" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="K92" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="K92" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="L92" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B93" s="1">
         <v>17</v>
@@ -4455,15 +4498,15 @@
         <v>30</v>
       </c>
       <c r="K93" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L93" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B94" s="1">
         <v>17</v>
@@ -4493,15 +4536,15 @@
         <v>29</v>
       </c>
       <c r="K94" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L94" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B95" s="1">
         <v>17</v>
@@ -4531,15 +4574,15 @@
         <v>40</v>
       </c>
       <c r="K95" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L95" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B96" s="1">
         <v>17</v>
@@ -4569,15 +4612,15 @@
         <v>24</v>
       </c>
       <c r="K96" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L96" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B97" s="1">
         <v>17</v>
@@ -4610,12 +4653,12 @@
         <v>52</v>
       </c>
       <c r="L97" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B98" s="1">
         <v>17</v>
@@ -4633,7 +4676,7 @@
         <v>51</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H98" s="1">
         <v>412</v>
@@ -4642,18 +4685,18 @@
         <v>0</v>
       </c>
       <c r="J98" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K98" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="K98" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="L98" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B99" s="1">
         <v>17</v>
@@ -4671,7 +4714,7 @@
         <v>51</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H99" s="1">
         <v>2645</v>
@@ -4680,18 +4723,18 @@
         <v>0</v>
       </c>
       <c r="J99" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K99" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L99" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B100" s="1">
         <v>18</v>
@@ -4724,12 +4767,12 @@
         <v>46</v>
       </c>
       <c r="L100" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B101" s="1">
         <v>18</v>
@@ -4762,12 +4805,12 @@
         <v>48</v>
       </c>
       <c r="L101" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B102" s="1">
         <v>18</v>
@@ -4800,12 +4843,12 @@
         <v>50</v>
       </c>
       <c r="L102" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B103" s="1">
         <v>18</v>
@@ -4838,12 +4881,12 @@
         <v>49</v>
       </c>
       <c r="L103" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B104" s="1">
         <v>18</v>
@@ -4876,12 +4919,12 @@
         <v>47</v>
       </c>
       <c r="L104" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B105" s="1">
         <v>18</v>
@@ -4914,12 +4957,12 @@
         <v>35</v>
       </c>
       <c r="L105" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B106" s="1">
         <v>18</v>
@@ -4949,15 +4992,15 @@
         <v>43</v>
       </c>
       <c r="K106" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L106" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B107" s="1">
         <v>18</v>
@@ -4975,7 +5018,7 @@
         <v>195</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H107">
         <v>49985</v>
@@ -4990,12 +5033,12 @@
         <v>37</v>
       </c>
       <c r="L107" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B108" s="1">
         <v>18</v>
@@ -5013,7 +5056,7 @@
         <v>195</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H108">
         <v>4222</v>
@@ -5022,18 +5065,18 @@
         <v>0</v>
       </c>
       <c r="J108" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K108" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L108" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B109" s="1">
         <v>18</v>
@@ -5063,15 +5106,15 @@
         <v>30</v>
       </c>
       <c r="K109" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L109" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B110" s="1">
         <v>18</v>
@@ -5089,7 +5132,7 @@
         <v>195</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H110">
         <v>5606</v>
@@ -5098,18 +5141,18 @@
         <v>0</v>
       </c>
       <c r="J110" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K110" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L110" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B111" s="1">
         <v>18</v>
@@ -5127,7 +5170,7 @@
         <v>195</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H111">
         <v>3354</v>
@@ -5136,18 +5179,18 @@
         <v>0</v>
       </c>
       <c r="J111" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K111" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L111" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B112" s="1">
         <v>18</v>
@@ -5165,7 +5208,7 @@
         <v>195</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H112">
         <v>2990</v>
@@ -5174,18 +5217,18 @@
         <v>0</v>
       </c>
       <c r="J112" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K112" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L112" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B113" s="1">
         <v>18</v>
@@ -5215,15 +5258,15 @@
         <v>24</v>
       </c>
       <c r="K113" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L113" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B114" s="1">
         <v>18</v>
@@ -5241,7 +5284,7 @@
         <v>195</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H114">
         <v>4162</v>
@@ -5250,18 +5293,18 @@
         <v>0</v>
       </c>
       <c r="J114" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K114" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L114" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B115" s="1">
         <v>18</v>
@@ -5279,7 +5322,7 @@
         <v>195</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H115">
         <v>3049</v>
@@ -5288,18 +5331,18 @@
         <v>0</v>
       </c>
       <c r="J115" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K115" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L115" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B116" s="1">
         <v>18</v>
@@ -5332,12 +5375,12 @@
         <v>51</v>
       </c>
       <c r="L116" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B117" s="1">
         <v>18</v>
@@ -5355,7 +5398,7 @@
         <v>195</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H117">
         <v>3839</v>
@@ -5364,18 +5407,18 @@
         <v>0</v>
       </c>
       <c r="J117" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="K117" t="s">
         <v>161</v>
       </c>
-      <c r="K117" t="s">
-        <v>162</v>
-      </c>
       <c r="L117" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B118" s="1">
         <v>18</v>
@@ -5393,7 +5436,7 @@
         <v>195</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H118">
         <v>5201</v>
@@ -5402,18 +5445,18 @@
         <v>0</v>
       </c>
       <c r="J118" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K118" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L118" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B119" s="1">
         <v>18</v>
@@ -5431,7 +5474,7 @@
         <v>195</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H119">
         <v>8235</v>
@@ -5440,18 +5483,18 @@
         <v>0</v>
       </c>
       <c r="J119" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="K119" t="s">
         <v>164</v>
       </c>
-      <c r="K119" t="s">
-        <v>165</v>
-      </c>
       <c r="L119" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B120" s="1">
         <v>18</v>
@@ -5469,7 +5512,7 @@
         <v>195</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H120">
         <v>14684</v>
@@ -5478,18 +5521,18 @@
         <v>0</v>
       </c>
       <c r="J120" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="K120" t="s">
         <v>135</v>
       </c>
-      <c r="K120" t="s">
-        <v>136</v>
-      </c>
       <c r="L120" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B121" s="1">
         <v>18</v>
@@ -5507,7 +5550,7 @@
         <v>195</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H121">
         <v>2192</v>
@@ -5516,18 +5559,18 @@
         <v>0</v>
       </c>
       <c r="J121" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="K121" t="s">
         <v>166</v>
       </c>
-      <c r="K121" t="s">
-        <v>167</v>
-      </c>
       <c r="L121" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B122" s="1">
         <v>18</v>
@@ -5557,15 +5600,15 @@
         <v>29</v>
       </c>
       <c r="K122" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L122" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B123" s="1">
         <v>18</v>
@@ -5583,7 +5626,7 @@
         <v>195</v>
       </c>
       <c r="G123" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H123">
         <v>6154</v>
@@ -5592,18 +5635,18 @@
         <v>0</v>
       </c>
       <c r="J123" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K123" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L123" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B124" s="1">
         <v>18</v>
@@ -5621,7 +5664,7 @@
         <v>195</v>
       </c>
       <c r="G124" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H124">
         <v>6364</v>
@@ -5630,18 +5673,18 @@
         <v>0</v>
       </c>
       <c r="J124" t="s">
+        <v>169</v>
+      </c>
+      <c r="K124" t="s">
         <v>170</v>
       </c>
-      <c r="K124" t="s">
-        <v>171</v>
-      </c>
       <c r="L124" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B125" s="1">
         <v>18</v>
@@ -5674,12 +5717,12 @@
         <v>52</v>
       </c>
       <c r="L125" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B126" s="1">
         <v>18</v>
@@ -5697,7 +5740,7 @@
         <v>195</v>
       </c>
       <c r="G126" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H126">
         <v>14799</v>
@@ -5706,18 +5749,18 @@
         <v>0</v>
       </c>
       <c r="J126" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K126" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L126" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B127" s="1">
         <v>18</v>
@@ -5735,7 +5778,7 @@
         <v>195</v>
       </c>
       <c r="G127" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H127">
         <v>45177</v>
@@ -5744,18 +5787,18 @@
         <v>0</v>
       </c>
       <c r="J127" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K127" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L127" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B128" s="1">
         <v>18</v>
@@ -5785,15 +5828,15 @@
         <v>40</v>
       </c>
       <c r="K128" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L128" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B129" s="1">
         <v>20</v>
@@ -5826,12 +5869,12 @@
         <v>46</v>
       </c>
       <c r="L129" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B130" s="1">
         <v>20</v>
@@ -5864,12 +5907,12 @@
         <v>48</v>
       </c>
       <c r="L130" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B131" s="1">
         <v>20</v>
@@ -5902,12 +5945,12 @@
         <v>50</v>
       </c>
       <c r="L131" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B132" s="1">
         <v>20</v>
@@ -5940,12 +5983,12 @@
         <v>49</v>
       </c>
       <c r="L132" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B133" s="1">
         <v>20</v>
@@ -5978,12 +6021,12 @@
         <v>47</v>
       </c>
       <c r="L133" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B134" s="1">
         <v>20</v>
@@ -6016,12 +6059,12 @@
         <v>35</v>
       </c>
       <c r="L134" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B135" s="1">
         <v>20</v>
@@ -6039,7 +6082,7 @@
         <v>69</v>
       </c>
       <c r="G135" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H135">
         <v>79301</v>
@@ -6048,18 +6091,18 @@
         <v>4</v>
       </c>
       <c r="J135" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K135" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L135" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B136" s="1">
         <v>20</v>
@@ -6089,15 +6132,15 @@
         <v>43</v>
       </c>
       <c r="K136" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L136" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B137" s="1">
         <v>20</v>
@@ -6115,7 +6158,7 @@
         <v>69</v>
       </c>
       <c r="G137" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H137">
         <v>8190</v>
@@ -6130,12 +6173,12 @@
         <v>37</v>
       </c>
       <c r="L137" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B138" s="1">
         <v>20</v>
@@ -6165,15 +6208,15 @@
         <v>40</v>
       </c>
       <c r="K138" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L138" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B139" s="1">
         <v>20</v>
@@ -6191,7 +6234,7 @@
         <v>69</v>
       </c>
       <c r="G139" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H139">
         <v>1692</v>
@@ -6200,18 +6243,18 @@
         <v>0</v>
       </c>
       <c r="J139" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K139" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L139" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B140" s="1">
         <v>20</v>
@@ -6244,12 +6287,12 @@
         <v>51</v>
       </c>
       <c r="L140" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B141" s="1">
         <v>20</v>
@@ -6279,15 +6322,15 @@
         <v>29</v>
       </c>
       <c r="K141" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L141" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B142" s="1">
         <v>20</v>
@@ -6317,15 +6360,15 @@
         <v>24</v>
       </c>
       <c r="K142" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L142" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B143" s="1">
         <v>20</v>
@@ -6358,12 +6401,12 @@
         <v>52</v>
       </c>
       <c r="L143" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B144" s="1">
         <v>20</v>
@@ -6381,7 +6424,7 @@
         <v>69</v>
       </c>
       <c r="G144" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H144">
         <v>4215</v>
@@ -6390,14 +6433,556 @@
         <v>0</v>
       </c>
       <c r="J144" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K144" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L144" s="2" t="s">
-        <v>173</v>
-      </c>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A145" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B145" s="1">
+        <v>19</v>
+      </c>
+      <c r="C145">
+        <v>6064738</v>
+      </c>
+      <c r="D145">
+        <v>3657881</v>
+      </c>
+      <c r="E145">
+        <v>3623799</v>
+      </c>
+      <c r="F145" s="1">
+        <v>146</v>
+      </c>
+      <c r="G145" t="s">
+        <v>14</v>
+      </c>
+      <c r="H145">
+        <v>1211418</v>
+      </c>
+      <c r="I145" s="1">
+        <v>57</v>
+      </c>
+      <c r="J145" t="s">
+        <v>14</v>
+      </c>
+      <c r="K145" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L145" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A146" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B146" s="1">
+        <v>19</v>
+      </c>
+      <c r="C146">
+        <v>6064738</v>
+      </c>
+      <c r="D146">
+        <v>3657881</v>
+      </c>
+      <c r="E146">
+        <v>3623799</v>
+      </c>
+      <c r="F146" s="1">
+        <v>146</v>
+      </c>
+      <c r="G146" t="s">
+        <v>11</v>
+      </c>
+      <c r="H146">
+        <v>1017276</v>
+      </c>
+      <c r="I146" s="1">
+        <v>47</v>
+      </c>
+      <c r="J146" t="s">
+        <v>11</v>
+      </c>
+      <c r="K146" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="L146" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A147" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B147" s="1">
+        <v>19</v>
+      </c>
+      <c r="C147">
+        <v>6064738</v>
+      </c>
+      <c r="D147">
+        <v>3657881</v>
+      </c>
+      <c r="E147">
+        <v>3623799</v>
+      </c>
+      <c r="F147" s="1">
+        <v>146</v>
+      </c>
+      <c r="G147" t="s">
+        <v>16</v>
+      </c>
+      <c r="H147">
+        <v>526923</v>
+      </c>
+      <c r="I147" s="1">
+        <v>24</v>
+      </c>
+      <c r="J147" t="s">
+        <v>36</v>
+      </c>
+      <c r="K147" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L147" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A148" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B148" s="1">
+        <v>19</v>
+      </c>
+      <c r="C148">
+        <v>6064738</v>
+      </c>
+      <c r="D148">
+        <v>3657881</v>
+      </c>
+      <c r="E148">
+        <v>3623799</v>
+      </c>
+      <c r="F148" s="1">
+        <v>146</v>
+      </c>
+      <c r="G148" t="s">
+        <v>15</v>
+      </c>
+      <c r="H148">
+        <v>170298</v>
+      </c>
+      <c r="I148" s="1">
+        <v>18</v>
+      </c>
+      <c r="J148" t="s">
+        <v>15</v>
+      </c>
+      <c r="K148" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L148" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A149" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B149" s="1">
+        <v>19</v>
+      </c>
+      <c r="C149">
+        <v>6064738</v>
+      </c>
+      <c r="D149">
+        <v>3657881</v>
+      </c>
+      <c r="E149">
+        <v>3623799</v>
+      </c>
+      <c r="F149" s="1">
+        <v>146</v>
+      </c>
+      <c r="G149" t="s">
+        <v>12</v>
+      </c>
+      <c r="H149">
+        <v>396839</v>
+      </c>
+      <c r="I149" s="1">
+        <v>0</v>
+      </c>
+      <c r="J149" t="s">
+        <v>12</v>
+      </c>
+      <c r="K149" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L149" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A150" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B150" s="1">
+        <v>19</v>
+      </c>
+      <c r="C150">
+        <v>6064738</v>
+      </c>
+      <c r="D150">
+        <v>3657881</v>
+      </c>
+      <c r="E150">
+        <v>3623799</v>
+      </c>
+      <c r="F150" s="1">
+        <v>146</v>
+      </c>
+      <c r="G150" t="s">
+        <v>13</v>
+      </c>
+      <c r="H150">
+        <v>98585</v>
+      </c>
+      <c r="I150" s="1">
+        <v>0</v>
+      </c>
+      <c r="J150" t="s">
+        <v>180</v>
+      </c>
+      <c r="K150" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="L150" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A151" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B151" s="1">
+        <v>19</v>
+      </c>
+      <c r="C151">
+        <v>6064738</v>
+      </c>
+      <c r="D151">
+        <v>3657881</v>
+      </c>
+      <c r="E151">
+        <v>3623799</v>
+      </c>
+      <c r="F151" s="1">
+        <v>146</v>
+      </c>
+      <c r="G151" t="s">
+        <v>18</v>
+      </c>
+      <c r="H151">
+        <v>36603</v>
+      </c>
+      <c r="I151" s="1">
+        <v>0</v>
+      </c>
+      <c r="J151" t="s">
+        <v>18</v>
+      </c>
+      <c r="K151" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="L151" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A152" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B152" s="1">
+        <v>19</v>
+      </c>
+      <c r="C152">
+        <v>6064738</v>
+      </c>
+      <c r="D152">
+        <v>3657881</v>
+      </c>
+      <c r="E152">
+        <v>3623799</v>
+      </c>
+      <c r="F152" s="1">
+        <v>146</v>
+      </c>
+      <c r="G152" t="s">
+        <v>190</v>
+      </c>
+      <c r="H152">
+        <v>30453</v>
+      </c>
+      <c r="I152" s="1">
+        <v>0</v>
+      </c>
+      <c r="J152" t="s">
+        <v>37</v>
+      </c>
+      <c r="K152" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="L152" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A153" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B153" s="1">
+        <v>19</v>
+      </c>
+      <c r="C153">
+        <v>6064738</v>
+      </c>
+      <c r="D153">
+        <v>3657881</v>
+      </c>
+      <c r="E153">
+        <v>3623799</v>
+      </c>
+      <c r="F153" s="1">
+        <v>146</v>
+      </c>
+      <c r="G153" t="s">
+        <v>29</v>
+      </c>
+      <c r="H153">
+        <v>6528</v>
+      </c>
+      <c r="I153" s="1">
+        <v>0</v>
+      </c>
+      <c r="J153" t="s">
+        <v>181</v>
+      </c>
+      <c r="K153" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="L153" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A154" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B154" s="1">
+        <v>19</v>
+      </c>
+      <c r="C154">
+        <v>6064738</v>
+      </c>
+      <c r="D154">
+        <v>3657881</v>
+      </c>
+      <c r="E154">
+        <v>3623799</v>
+      </c>
+      <c r="F154" s="1">
+        <v>146</v>
+      </c>
+      <c r="G154" t="s">
+        <v>21</v>
+      </c>
+      <c r="H154">
+        <v>34159</v>
+      </c>
+      <c r="I154" s="1">
+        <v>0</v>
+      </c>
+      <c r="J154" t="s">
+        <v>40</v>
+      </c>
+      <c r="K154" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="L154" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A155" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B155" s="1">
+        <v>19</v>
+      </c>
+      <c r="C155">
+        <v>6064738</v>
+      </c>
+      <c r="D155">
+        <v>3657881</v>
+      </c>
+      <c r="E155">
+        <v>3623799</v>
+      </c>
+      <c r="F155" s="1">
+        <v>146</v>
+      </c>
+      <c r="G155" t="s">
+        <v>24</v>
+      </c>
+      <c r="H155">
+        <v>10673</v>
+      </c>
+      <c r="I155" s="1">
+        <v>0</v>
+      </c>
+      <c r="J155" t="s">
+        <v>24</v>
+      </c>
+      <c r="K155" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L155" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A156" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B156" s="1">
+        <v>19</v>
+      </c>
+      <c r="C156">
+        <v>6064738</v>
+      </c>
+      <c r="D156">
+        <v>3657881</v>
+      </c>
+      <c r="E156">
+        <v>3623799</v>
+      </c>
+      <c r="F156" s="1">
+        <v>146</v>
+      </c>
+      <c r="G156" t="s">
+        <v>19</v>
+      </c>
+      <c r="H156">
+        <v>53139</v>
+      </c>
+      <c r="I156" s="1">
+        <v>0</v>
+      </c>
+      <c r="J156" t="s">
+        <v>38</v>
+      </c>
+      <c r="K156" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="L156" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A157" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B157" s="1">
+        <v>19</v>
+      </c>
+      <c r="C157">
+        <v>6064738</v>
+      </c>
+      <c r="D157">
+        <v>3657881</v>
+      </c>
+      <c r="E157">
+        <v>3623799</v>
+      </c>
+      <c r="F157" s="1">
+        <v>146</v>
+      </c>
+      <c r="G157" t="s">
+        <v>25</v>
+      </c>
+      <c r="H157">
+        <v>14242</v>
+      </c>
+      <c r="I157" s="1">
+        <v>0</v>
+      </c>
+      <c r="J157" t="s">
+        <v>43</v>
+      </c>
+      <c r="K157" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="L157" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A158" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B158" s="1">
+        <v>19</v>
+      </c>
+      <c r="C158">
+        <v>6064738</v>
+      </c>
+      <c r="D158">
+        <v>3657881</v>
+      </c>
+      <c r="E158">
+        <v>3623799</v>
+      </c>
+      <c r="F158" s="1">
+        <v>146</v>
+      </c>
+      <c r="G158" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H158">
+        <v>16663</v>
+      </c>
+      <c r="I158" s="1">
+        <v>0</v>
+      </c>
+      <c r="J158" t="s">
+        <v>79</v>
+      </c>
+      <c r="K158" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="L158" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G159" s="1"/>
+      <c r="K159" s="1"/>
+    </row>
+    <row r="167" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G167" s="5"/>
+      <c r="H167" s="5"/>
+      <c r="J167" s="1"/>
+      <c r="K167" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add BY2023 election and gov and HE2023 election
</commit_message>
<xml_diff>
--- a/inst/extdata/additional_elecdata.xlsx
+++ b/inst/extdata/additional_elecdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\add\bundeslaendeR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6503A922-29AA-46E9-9815-0BCA8FF5D770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D30A716-FA96-463D-B4C2-36C464368D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="224">
   <si>
     <t>state</t>
   </si>
@@ -637,6 +637,75 @@
   </si>
   <si>
     <t>2023-05-14</t>
+  </si>
+  <si>
+    <t>BY</t>
+  </si>
+  <si>
+    <t>2023-10-08</t>
+  </si>
+  <si>
+    <t>CSU</t>
+  </si>
+  <si>
+    <t>FW-BY</t>
+  </si>
+  <si>
+    <t>BP</t>
+  </si>
+  <si>
+    <t>VPartei3</t>
+  </si>
+  <si>
+    <t>V-Partei³</t>
+  </si>
+  <si>
+    <t>PdH</t>
+  </si>
+  <si>
+    <t>Christlich Soziale Union in Bayern e.V.</t>
+  </si>
+  <si>
+    <t>Bayernpartei</t>
+  </si>
+  <si>
+    <t>V-Partei³ – Partei für Veränderung, Vegetarier und Veganer</t>
+  </si>
+  <si>
+    <t>HE</t>
+  </si>
+  <si>
+    <t>FW-HE</t>
+  </si>
+  <si>
+    <t>ABG</t>
+  </si>
+  <si>
+    <t>APPD</t>
+  </si>
+  <si>
+    <t>DNM</t>
+  </si>
+  <si>
+    <t>WKH</t>
+  </si>
+  <si>
+    <t>DIE NEUE MITTE</t>
+  </si>
+  <si>
+    <t>KLIMALISTE WÄHLERLISTE</t>
+  </si>
+  <si>
+    <t>V-Partei³ - Partei für Veränderung, Vegetarier und Veganer</t>
+  </si>
+  <si>
+    <t>Aktion Bürger für Gerechtigkeit</t>
+  </si>
+  <si>
+    <t>Anarchistische Pogo-Partei Deutschlands</t>
+  </si>
+  <si>
+    <t>Wählerliste Klimaliste Hessen</t>
   </si>
 </sst>
 </file>
@@ -685,7 +754,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -693,6 +762,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -973,11 +1045,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L207"/>
+  <dimension ref="A1:L243"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A185" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E199" sqref="E199"/>
+      <pane ySplit="1" topLeftCell="A209" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G248" sqref="G248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -8862,6 +8934,1374 @@
         <v>200</v>
       </c>
     </row>
+    <row r="208" spans="1:12">
+      <c r="A208" t="s">
+        <v>201</v>
+      </c>
+      <c r="B208">
+        <v>19</v>
+      </c>
+      <c r="C208">
+        <v>9430600</v>
+      </c>
+      <c r="D208">
+        <v>6895807</v>
+      </c>
+      <c r="E208">
+        <v>13658782</v>
+      </c>
+      <c r="F208">
+        <v>203</v>
+      </c>
+      <c r="G208" t="s">
+        <v>203</v>
+      </c>
+      <c r="H208">
+        <v>5059571</v>
+      </c>
+      <c r="I208">
+        <v>85</v>
+      </c>
+      <c r="J208" t="s">
+        <v>203</v>
+      </c>
+      <c r="K208" t="s">
+        <v>209</v>
+      </c>
+      <c r="L208" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="209" spans="1:12">
+      <c r="A209" t="s">
+        <v>201</v>
+      </c>
+      <c r="B209">
+        <v>19</v>
+      </c>
+      <c r="C209">
+        <v>9430600</v>
+      </c>
+      <c r="D209">
+        <v>6895807</v>
+      </c>
+      <c r="E209">
+        <v>13658782</v>
+      </c>
+      <c r="F209">
+        <v>203</v>
+      </c>
+      <c r="G209" t="s">
+        <v>16</v>
+      </c>
+      <c r="H209">
+        <v>1972725</v>
+      </c>
+      <c r="I209">
+        <v>32</v>
+      </c>
+      <c r="J209" t="s">
+        <v>36</v>
+      </c>
+      <c r="K209" t="s">
+        <v>50</v>
+      </c>
+      <c r="L209" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="210" spans="1:12">
+      <c r="A210" t="s">
+        <v>201</v>
+      </c>
+      <c r="B210">
+        <v>19</v>
+      </c>
+      <c r="C210">
+        <v>9430600</v>
+      </c>
+      <c r="D210">
+        <v>6895807</v>
+      </c>
+      <c r="E210">
+        <v>13658782</v>
+      </c>
+      <c r="F210">
+        <v>203</v>
+      </c>
+      <c r="G210" t="s">
+        <v>204</v>
+      </c>
+      <c r="H210">
+        <v>2163849</v>
+      </c>
+      <c r="I210">
+        <v>37</v>
+      </c>
+      <c r="J210" t="s">
+        <v>37</v>
+      </c>
+      <c r="K210" t="s">
+        <v>37</v>
+      </c>
+      <c r="L210" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="211" spans="1:12">
+      <c r="A211" t="s">
+        <v>201</v>
+      </c>
+      <c r="B211">
+        <v>19</v>
+      </c>
+      <c r="C211">
+        <v>9430600</v>
+      </c>
+      <c r="D211">
+        <v>6895807</v>
+      </c>
+      <c r="E211">
+        <v>13658782</v>
+      </c>
+      <c r="F211">
+        <v>203</v>
+      </c>
+      <c r="G211" t="s">
+        <v>12</v>
+      </c>
+      <c r="H211">
+        <v>2000435</v>
+      </c>
+      <c r="I211">
+        <v>32</v>
+      </c>
+      <c r="J211" t="s">
+        <v>12</v>
+      </c>
+      <c r="K211" t="s">
+        <v>47</v>
+      </c>
+      <c r="L211" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="212" spans="1:12">
+      <c r="A212" t="s">
+        <v>201</v>
+      </c>
+      <c r="B212">
+        <v>19</v>
+      </c>
+      <c r="C212">
+        <v>9430600</v>
+      </c>
+      <c r="D212">
+        <v>6895807</v>
+      </c>
+      <c r="E212">
+        <v>13658782</v>
+      </c>
+      <c r="F212">
+        <v>203</v>
+      </c>
+      <c r="G212" t="s">
+        <v>14</v>
+      </c>
+      <c r="H212">
+        <v>1140753</v>
+      </c>
+      <c r="I212">
+        <v>17</v>
+      </c>
+      <c r="J212" t="s">
+        <v>14</v>
+      </c>
+      <c r="K212" t="s">
+        <v>48</v>
+      </c>
+      <c r="L212" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="213" spans="1:12">
+      <c r="A213" t="s">
+        <v>201</v>
+      </c>
+      <c r="B213">
+        <v>19</v>
+      </c>
+      <c r="C213">
+        <v>9430600</v>
+      </c>
+      <c r="D213">
+        <v>6895807</v>
+      </c>
+      <c r="E213">
+        <v>13658782</v>
+      </c>
+      <c r="F213">
+        <v>203</v>
+      </c>
+      <c r="G213" t="s">
+        <v>15</v>
+      </c>
+      <c r="H213">
+        <v>413887</v>
+      </c>
+      <c r="I213">
+        <v>0</v>
+      </c>
+      <c r="J213" t="s">
+        <v>15</v>
+      </c>
+      <c r="K213" t="s">
+        <v>49</v>
+      </c>
+      <c r="L213" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="214" spans="1:12">
+      <c r="A214" t="s">
+        <v>201</v>
+      </c>
+      <c r="B214">
+        <v>19</v>
+      </c>
+      <c r="C214">
+        <v>9430600</v>
+      </c>
+      <c r="D214">
+        <v>6895807</v>
+      </c>
+      <c r="E214">
+        <v>13658782</v>
+      </c>
+      <c r="F214">
+        <v>203</v>
+      </c>
+      <c r="G214" t="s">
+        <v>13</v>
+      </c>
+      <c r="H214">
+        <v>200878</v>
+      </c>
+      <c r="I214">
+        <v>0</v>
+      </c>
+      <c r="J214" t="s">
+        <v>35</v>
+      </c>
+      <c r="K214" t="s">
+        <v>35</v>
+      </c>
+      <c r="L214" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="215" spans="1:12">
+      <c r="A215" t="s">
+        <v>201</v>
+      </c>
+      <c r="B215">
+        <v>19</v>
+      </c>
+      <c r="C215">
+        <v>9430600</v>
+      </c>
+      <c r="D215">
+        <v>6895807</v>
+      </c>
+      <c r="E215">
+        <v>13658782</v>
+      </c>
+      <c r="F215">
+        <v>203</v>
+      </c>
+      <c r="G215" t="s">
+        <v>205</v>
+      </c>
+      <c r="H215">
+        <v>129480</v>
+      </c>
+      <c r="I215">
+        <v>0</v>
+      </c>
+      <c r="J215" t="s">
+        <v>205</v>
+      </c>
+      <c r="K215" t="s">
+        <v>210</v>
+      </c>
+      <c r="L215" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="216" spans="1:12">
+      <c r="A216" t="s">
+        <v>201</v>
+      </c>
+      <c r="B216">
+        <v>19</v>
+      </c>
+      <c r="C216">
+        <v>9430600</v>
+      </c>
+      <c r="D216">
+        <v>6895807</v>
+      </c>
+      <c r="E216">
+        <v>13658782</v>
+      </c>
+      <c r="F216">
+        <v>203</v>
+      </c>
+      <c r="G216" t="s">
+        <v>30</v>
+      </c>
+      <c r="H216">
+        <v>245224</v>
+      </c>
+      <c r="I216">
+        <v>0</v>
+      </c>
+      <c r="J216" t="s">
+        <v>30</v>
+      </c>
+      <c r="K216" t="s">
+        <v>60</v>
+      </c>
+      <c r="L216" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="217" spans="1:12">
+      <c r="A217" t="s">
+        <v>201</v>
+      </c>
+      <c r="B217">
+        <v>19</v>
+      </c>
+      <c r="C217">
+        <v>9430600</v>
+      </c>
+      <c r="D217">
+        <v>6895807</v>
+      </c>
+      <c r="E217">
+        <v>13658782</v>
+      </c>
+      <c r="F217">
+        <v>203</v>
+      </c>
+      <c r="G217" t="s">
+        <v>21</v>
+      </c>
+      <c r="H217">
+        <v>64154</v>
+      </c>
+      <c r="I217">
+        <v>0</v>
+      </c>
+      <c r="J217" t="s">
+        <v>40</v>
+      </c>
+      <c r="K217" t="s">
+        <v>191</v>
+      </c>
+      <c r="L217" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="218" spans="1:12">
+      <c r="A218" t="s">
+        <v>201</v>
+      </c>
+      <c r="B218">
+        <v>19</v>
+      </c>
+      <c r="C218">
+        <v>9430600</v>
+      </c>
+      <c r="D218">
+        <v>6895807</v>
+      </c>
+      <c r="E218">
+        <v>13658782</v>
+      </c>
+      <c r="F218">
+        <v>203</v>
+      </c>
+      <c r="G218" t="s">
+        <v>19</v>
+      </c>
+      <c r="H218">
+        <v>69792</v>
+      </c>
+      <c r="I218">
+        <v>0</v>
+      </c>
+      <c r="J218" t="s">
+        <v>38</v>
+      </c>
+      <c r="K218" t="s">
+        <v>52</v>
+      </c>
+      <c r="L218" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="219" spans="1:12">
+      <c r="A219" t="s">
+        <v>201</v>
+      </c>
+      <c r="B219">
+        <v>19</v>
+      </c>
+      <c r="C219">
+        <v>9430600</v>
+      </c>
+      <c r="D219">
+        <v>6895807</v>
+      </c>
+      <c r="E219">
+        <v>13658782</v>
+      </c>
+      <c r="F219">
+        <v>203</v>
+      </c>
+      <c r="G219" t="s">
+        <v>206</v>
+      </c>
+      <c r="H219">
+        <v>22825</v>
+      </c>
+      <c r="I219">
+        <v>0</v>
+      </c>
+      <c r="J219" t="s">
+        <v>207</v>
+      </c>
+      <c r="K219" t="s">
+        <v>211</v>
+      </c>
+      <c r="L219" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="220" spans="1:12">
+      <c r="A220" t="s">
+        <v>201</v>
+      </c>
+      <c r="B220">
+        <v>19</v>
+      </c>
+      <c r="C220">
+        <v>9430600</v>
+      </c>
+      <c r="D220">
+        <v>6895807</v>
+      </c>
+      <c r="E220">
+        <v>13658782</v>
+      </c>
+      <c r="F220">
+        <v>203</v>
+      </c>
+      <c r="G220" t="s">
+        <v>29</v>
+      </c>
+      <c r="H220">
+        <v>14026</v>
+      </c>
+      <c r="I220">
+        <v>0</v>
+      </c>
+      <c r="J220" t="s">
+        <v>208</v>
+      </c>
+      <c r="K220" t="s">
+        <v>59</v>
+      </c>
+      <c r="L220" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="221" spans="1:12">
+      <c r="A221" t="s">
+        <v>201</v>
+      </c>
+      <c r="B221">
+        <v>19</v>
+      </c>
+      <c r="C221">
+        <v>9430600</v>
+      </c>
+      <c r="D221">
+        <v>6895807</v>
+      </c>
+      <c r="E221">
+        <v>13658782</v>
+      </c>
+      <c r="F221">
+        <v>203</v>
+      </c>
+      <c r="G221" t="s">
+        <v>18</v>
+      </c>
+      <c r="H221">
+        <v>119489</v>
+      </c>
+      <c r="I221">
+        <v>0</v>
+      </c>
+      <c r="J221" t="s">
+        <v>18</v>
+      </c>
+      <c r="K221" t="s">
+        <v>51</v>
+      </c>
+      <c r="L221" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="222" spans="1:12">
+      <c r="A222" t="s">
+        <v>201</v>
+      </c>
+      <c r="B222">
+        <v>19</v>
+      </c>
+      <c r="C222">
+        <v>9430600</v>
+      </c>
+      <c r="D222">
+        <v>6895807</v>
+      </c>
+      <c r="E222">
+        <v>13658782</v>
+      </c>
+      <c r="F222">
+        <v>203</v>
+      </c>
+      <c r="G222" t="s">
+        <v>79</v>
+      </c>
+      <c r="H222">
+        <v>41694</v>
+      </c>
+      <c r="I222">
+        <v>0</v>
+      </c>
+      <c r="J222" t="s">
+        <v>79</v>
+      </c>
+      <c r="K222" t="s">
+        <v>109</v>
+      </c>
+      <c r="L222" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="223" spans="1:12">
+      <c r="A223" t="s">
+        <v>212</v>
+      </c>
+      <c r="B223">
+        <v>21</v>
+      </c>
+      <c r="C223">
+        <v>4332235</v>
+      </c>
+      <c r="D223">
+        <v>2858313</v>
+      </c>
+      <c r="E223">
+        <v>2813313</v>
+      </c>
+      <c r="F223">
+        <v>133</v>
+      </c>
+      <c r="G223" t="s">
+        <v>11</v>
+      </c>
+      <c r="H223">
+        <v>972876</v>
+      </c>
+      <c r="I223">
+        <v>52</v>
+      </c>
+      <c r="J223" t="s">
+        <v>11</v>
+      </c>
+      <c r="K223" t="s">
+        <v>46</v>
+      </c>
+      <c r="L223" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="224" spans="1:12">
+      <c r="A224" t="s">
+        <v>212</v>
+      </c>
+      <c r="B224">
+        <v>21</v>
+      </c>
+      <c r="C224">
+        <v>4332235</v>
+      </c>
+      <c r="D224">
+        <v>2858313</v>
+      </c>
+      <c r="E224">
+        <v>2813313</v>
+      </c>
+      <c r="F224">
+        <v>133</v>
+      </c>
+      <c r="G224" t="s">
+        <v>16</v>
+      </c>
+      <c r="H224">
+        <v>416035</v>
+      </c>
+      <c r="I224">
+        <v>22</v>
+      </c>
+      <c r="J224" t="s">
+        <v>36</v>
+      </c>
+      <c r="K224" t="s">
+        <v>50</v>
+      </c>
+      <c r="L224" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="225" spans="1:12">
+      <c r="A225" t="s">
+        <v>212</v>
+      </c>
+      <c r="B225">
+        <v>21</v>
+      </c>
+      <c r="C225">
+        <v>4332235</v>
+      </c>
+      <c r="D225">
+        <v>2858313</v>
+      </c>
+      <c r="E225">
+        <v>2813313</v>
+      </c>
+      <c r="F225">
+        <v>133</v>
+      </c>
+      <c r="G225" t="s">
+        <v>14</v>
+      </c>
+      <c r="H225">
+        <v>424587</v>
+      </c>
+      <c r="I225">
+        <v>23</v>
+      </c>
+      <c r="J225" t="s">
+        <v>14</v>
+      </c>
+      <c r="K225" t="s">
+        <v>48</v>
+      </c>
+      <c r="L225" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="226" spans="1:12">
+      <c r="A226" t="s">
+        <v>212</v>
+      </c>
+      <c r="B226">
+        <v>21</v>
+      </c>
+      <c r="C226">
+        <v>4332235</v>
+      </c>
+      <c r="D226">
+        <v>2858313</v>
+      </c>
+      <c r="E226">
+        <v>2813313</v>
+      </c>
+      <c r="F226">
+        <v>133</v>
+      </c>
+      <c r="G226" t="s">
+        <v>12</v>
+      </c>
+      <c r="H226">
+        <v>518763</v>
+      </c>
+      <c r="I226">
+        <v>28</v>
+      </c>
+      <c r="J226" t="s">
+        <v>12</v>
+      </c>
+      <c r="K226" t="s">
+        <v>47</v>
+      </c>
+      <c r="L226" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="227" spans="1:12">
+      <c r="A227" t="s">
+        <v>212</v>
+      </c>
+      <c r="B227">
+        <v>21</v>
+      </c>
+      <c r="C227">
+        <v>4332235</v>
+      </c>
+      <c r="D227">
+        <v>2858313</v>
+      </c>
+      <c r="E227">
+        <v>2813313</v>
+      </c>
+      <c r="F227">
+        <v>133</v>
+      </c>
+      <c r="G227" t="s">
+        <v>15</v>
+      </c>
+      <c r="H227">
+        <v>141644</v>
+      </c>
+      <c r="I227">
+        <v>8</v>
+      </c>
+      <c r="J227" t="s">
+        <v>15</v>
+      </c>
+      <c r="K227" t="s">
+        <v>49</v>
+      </c>
+      <c r="L227" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="228" spans="1:12">
+      <c r="A228" t="s">
+        <v>212</v>
+      </c>
+      <c r="B228">
+        <v>21</v>
+      </c>
+      <c r="C228">
+        <v>4332235</v>
+      </c>
+      <c r="D228">
+        <v>2858313</v>
+      </c>
+      <c r="E228">
+        <v>2813313</v>
+      </c>
+      <c r="F228">
+        <v>133</v>
+      </c>
+      <c r="G228" t="s">
+        <v>13</v>
+      </c>
+      <c r="H228">
+        <v>86842</v>
+      </c>
+      <c r="I228">
+        <v>0</v>
+      </c>
+      <c r="J228" t="s">
+        <v>35</v>
+      </c>
+      <c r="K228" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L228" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="229" spans="1:12">
+      <c r="A229" t="s">
+        <v>212</v>
+      </c>
+      <c r="B229">
+        <v>21</v>
+      </c>
+      <c r="C229">
+        <v>4332235</v>
+      </c>
+      <c r="D229">
+        <v>2858313</v>
+      </c>
+      <c r="E229">
+        <v>2813313</v>
+      </c>
+      <c r="F229">
+        <v>133</v>
+      </c>
+      <c r="G229" t="s">
+        <v>213</v>
+      </c>
+      <c r="H229">
+        <v>98283</v>
+      </c>
+      <c r="I229">
+        <v>0</v>
+      </c>
+      <c r="J229" t="s">
+        <v>37</v>
+      </c>
+      <c r="K229" t="s">
+        <v>37</v>
+      </c>
+      <c r="L229" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="230" spans="1:12">
+      <c r="A230" t="s">
+        <v>212</v>
+      </c>
+      <c r="B230">
+        <v>21</v>
+      </c>
+      <c r="C230">
+        <v>4332235</v>
+      </c>
+      <c r="D230">
+        <v>2858313</v>
+      </c>
+      <c r="E230">
+        <v>2813313</v>
+      </c>
+      <c r="F230">
+        <v>133</v>
+      </c>
+      <c r="G230" t="s">
+        <v>19</v>
+      </c>
+      <c r="H230">
+        <v>43341</v>
+      </c>
+      <c r="I230">
+        <v>0</v>
+      </c>
+      <c r="J230" t="s">
+        <v>38</v>
+      </c>
+      <c r="K230" t="s">
+        <v>52</v>
+      </c>
+      <c r="L230" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="231" spans="1:12">
+      <c r="A231" t="s">
+        <v>212</v>
+      </c>
+      <c r="B231">
+        <v>21</v>
+      </c>
+      <c r="C231">
+        <v>4332235</v>
+      </c>
+      <c r="D231">
+        <v>2858313</v>
+      </c>
+      <c r="E231">
+        <v>2813313</v>
+      </c>
+      <c r="F231">
+        <v>133</v>
+      </c>
+      <c r="G231" t="s">
+        <v>21</v>
+      </c>
+      <c r="H231">
+        <v>23678</v>
+      </c>
+      <c r="I231">
+        <v>0</v>
+      </c>
+      <c r="J231" t="s">
+        <v>40</v>
+      </c>
+      <c r="K231" t="s">
+        <v>191</v>
+      </c>
+      <c r="L231" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="232" spans="1:12">
+      <c r="A232" t="s">
+        <v>212</v>
+      </c>
+      <c r="B232">
+        <v>21</v>
+      </c>
+      <c r="C232">
+        <v>4332235</v>
+      </c>
+      <c r="D232">
+        <v>2858313</v>
+      </c>
+      <c r="E232">
+        <v>2813313</v>
+      </c>
+      <c r="F232">
+        <v>133</v>
+      </c>
+      <c r="G232" t="s">
+        <v>25</v>
+      </c>
+      <c r="H232">
+        <v>8618</v>
+      </c>
+      <c r="I232">
+        <v>0</v>
+      </c>
+      <c r="J232" t="s">
+        <v>43</v>
+      </c>
+      <c r="K232" t="s">
+        <v>56</v>
+      </c>
+      <c r="L232" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="233" spans="1:12">
+      <c r="A233" t="s">
+        <v>212</v>
+      </c>
+      <c r="B233">
+        <v>21</v>
+      </c>
+      <c r="C233">
+        <v>4332235</v>
+      </c>
+      <c r="D233">
+        <v>2858313</v>
+      </c>
+      <c r="E233">
+        <v>2813313</v>
+      </c>
+      <c r="F233">
+        <v>133</v>
+      </c>
+      <c r="G233" t="s">
+        <v>30</v>
+      </c>
+      <c r="H233">
+        <v>5906</v>
+      </c>
+      <c r="I233">
+        <v>0</v>
+      </c>
+      <c r="J233" t="s">
+        <v>30</v>
+      </c>
+      <c r="K233" t="s">
+        <v>60</v>
+      </c>
+      <c r="L233" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="234" spans="1:12">
+      <c r="A234" t="s">
+        <v>212</v>
+      </c>
+      <c r="B234">
+        <v>21</v>
+      </c>
+      <c r="C234">
+        <v>4332235</v>
+      </c>
+      <c r="D234">
+        <v>2858313</v>
+      </c>
+      <c r="E234">
+        <v>2813313</v>
+      </c>
+      <c r="F234">
+        <v>133</v>
+      </c>
+      <c r="G234" t="s">
+        <v>24</v>
+      </c>
+      <c r="H234">
+        <v>1506</v>
+      </c>
+      <c r="I234">
+        <v>0</v>
+      </c>
+      <c r="J234" t="s">
+        <v>198</v>
+      </c>
+      <c r="K234" t="s">
+        <v>199</v>
+      </c>
+      <c r="L234" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="235" spans="1:12">
+      <c r="A235" t="s">
+        <v>212</v>
+      </c>
+      <c r="B235">
+        <v>21</v>
+      </c>
+      <c r="C235">
+        <v>4332235</v>
+      </c>
+      <c r="D235">
+        <v>2858313</v>
+      </c>
+      <c r="E235">
+        <v>2813313</v>
+      </c>
+      <c r="F235">
+        <v>133</v>
+      </c>
+      <c r="G235" t="s">
+        <v>206</v>
+      </c>
+      <c r="H235">
+        <v>9472</v>
+      </c>
+      <c r="I235">
+        <v>0</v>
+      </c>
+      <c r="J235" t="s">
+        <v>207</v>
+      </c>
+      <c r="K235" t="s">
+        <v>220</v>
+      </c>
+      <c r="L235" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="236" spans="1:12">
+      <c r="A236" t="s">
+        <v>212</v>
+      </c>
+      <c r="B236">
+        <v>21</v>
+      </c>
+      <c r="C236">
+        <v>4332235</v>
+      </c>
+      <c r="D236">
+        <v>2858313</v>
+      </c>
+      <c r="E236">
+        <v>2813313</v>
+      </c>
+      <c r="F236">
+        <v>133</v>
+      </c>
+      <c r="G236" t="s">
+        <v>29</v>
+      </c>
+      <c r="H236">
+        <v>4262</v>
+      </c>
+      <c r="I236">
+        <v>0</v>
+      </c>
+      <c r="J236" t="s">
+        <v>208</v>
+      </c>
+      <c r="K236" t="s">
+        <v>59</v>
+      </c>
+      <c r="L236" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="237" spans="1:12">
+      <c r="A237" t="s">
+        <v>212</v>
+      </c>
+      <c r="B237">
+        <v>21</v>
+      </c>
+      <c r="C237">
+        <v>4332235</v>
+      </c>
+      <c r="D237">
+        <v>2858313</v>
+      </c>
+      <c r="E237">
+        <v>2813313</v>
+      </c>
+      <c r="F237">
+        <v>133</v>
+      </c>
+      <c r="G237" t="s">
+        <v>214</v>
+      </c>
+      <c r="H237">
+        <v>4442</v>
+      </c>
+      <c r="I237">
+        <v>0</v>
+      </c>
+      <c r="J237" t="s">
+        <v>214</v>
+      </c>
+      <c r="K237" t="s">
+        <v>221</v>
+      </c>
+      <c r="L237" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="238" spans="1:12">
+      <c r="A238" t="s">
+        <v>212</v>
+      </c>
+      <c r="B238">
+        <v>21</v>
+      </c>
+      <c r="C238">
+        <v>4332235</v>
+      </c>
+      <c r="D238">
+        <v>2858313</v>
+      </c>
+      <c r="E238">
+        <v>2813313</v>
+      </c>
+      <c r="F238">
+        <v>133</v>
+      </c>
+      <c r="G238" t="s">
+        <v>215</v>
+      </c>
+      <c r="H238">
+        <v>1929</v>
+      </c>
+      <c r="I238">
+        <v>0</v>
+      </c>
+      <c r="J238" t="s">
+        <v>215</v>
+      </c>
+      <c r="K238" t="s">
+        <v>222</v>
+      </c>
+      <c r="L238" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="239" spans="1:12">
+      <c r="A239" t="s">
+        <v>212</v>
+      </c>
+      <c r="B239">
+        <v>21</v>
+      </c>
+      <c r="C239">
+        <v>4332235</v>
+      </c>
+      <c r="D239">
+        <v>2858313</v>
+      </c>
+      <c r="E239">
+        <v>2813313</v>
+      </c>
+      <c r="F239">
+        <v>133</v>
+      </c>
+      <c r="G239" t="s">
+        <v>18</v>
+      </c>
+      <c r="H239">
+        <v>13707</v>
+      </c>
+      <c r="I239">
+        <v>0</v>
+      </c>
+      <c r="J239" t="s">
+        <v>18</v>
+      </c>
+      <c r="K239" t="s">
+        <v>51</v>
+      </c>
+      <c r="L239" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="240" spans="1:12">
+      <c r="A240" t="s">
+        <v>212</v>
+      </c>
+      <c r="B240">
+        <v>21</v>
+      </c>
+      <c r="C240">
+        <v>4332235</v>
+      </c>
+      <c r="D240">
+        <v>2858313</v>
+      </c>
+      <c r="E240">
+        <v>2813313</v>
+      </c>
+      <c r="F240">
+        <v>133</v>
+      </c>
+      <c r="G240" t="s">
+        <v>64</v>
+      </c>
+      <c r="H240">
+        <v>2229</v>
+      </c>
+      <c r="I240">
+        <v>0</v>
+      </c>
+      <c r="J240" t="s">
+        <v>64</v>
+      </c>
+      <c r="K240" t="s">
+        <v>95</v>
+      </c>
+      <c r="L240" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="241" spans="1:12">
+      <c r="A241" t="s">
+        <v>212</v>
+      </c>
+      <c r="B241">
+        <v>21</v>
+      </c>
+      <c r="C241">
+        <v>4332235</v>
+      </c>
+      <c r="D241">
+        <v>2858313</v>
+      </c>
+      <c r="E241">
+        <v>2813313</v>
+      </c>
+      <c r="F241">
+        <v>133</v>
+      </c>
+      <c r="G241" t="s">
+        <v>216</v>
+      </c>
+      <c r="H241">
+        <v>1369</v>
+      </c>
+      <c r="I241">
+        <v>0</v>
+      </c>
+      <c r="J241" t="s">
+        <v>218</v>
+      </c>
+      <c r="K241" t="s">
+        <v>218</v>
+      </c>
+      <c r="L241" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="242" spans="1:12">
+      <c r="A242" t="s">
+        <v>212</v>
+      </c>
+      <c r="B242">
+        <v>21</v>
+      </c>
+      <c r="C242">
+        <v>4332235</v>
+      </c>
+      <c r="D242">
+        <v>2858313</v>
+      </c>
+      <c r="E242">
+        <v>2813313</v>
+      </c>
+      <c r="F242">
+        <v>133</v>
+      </c>
+      <c r="G242" t="s">
+        <v>79</v>
+      </c>
+      <c r="H242">
+        <v>27612</v>
+      </c>
+      <c r="I242">
+        <v>0</v>
+      </c>
+      <c r="J242" t="s">
+        <v>79</v>
+      </c>
+      <c r="K242" t="s">
+        <v>109</v>
+      </c>
+      <c r="L242" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="243" spans="1:12">
+      <c r="A243" t="s">
+        <v>212</v>
+      </c>
+      <c r="B243">
+        <v>21</v>
+      </c>
+      <c r="C243">
+        <v>4332235</v>
+      </c>
+      <c r="D243">
+        <v>2858313</v>
+      </c>
+      <c r="E243">
+        <v>2813313</v>
+      </c>
+      <c r="F243">
+        <v>133</v>
+      </c>
+      <c r="G243" t="s">
+        <v>217</v>
+      </c>
+      <c r="H243">
+        <v>6212</v>
+      </c>
+      <c r="I243">
+        <v>0</v>
+      </c>
+      <c r="J243" t="s">
+        <v>219</v>
+      </c>
+      <c r="K243" t="s">
+        <v>223</v>
+      </c>
+      <c r="L243" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix ni 2022 and add he 2024 gov
</commit_message>
<xml_diff>
--- a/inst/extdata/additional_elecdata.xlsx
+++ b/inst/extdata/additional_elecdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\add\bundeslaendeR\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Git_Projekte\bundeslaendeR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D30A716-FA96-463D-B4C2-36C464368D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576801A1-176B-4427-8502-26E2FFEDFD64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1048,8 +1048,8 @@
   <dimension ref="A1:L243"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A209" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G248" sqref="G248"/>
+      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K148" sqref="K148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -6680,7 +6680,7 @@
         <v>170298</v>
       </c>
       <c r="I148">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="J148" t="s">
         <v>15</v>
@@ -6718,7 +6718,7 @@
         <v>396839</v>
       </c>
       <c r="I149">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="J149" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Update data from 2024 and 2025 and some minor changes to the codebook
</commit_message>
<xml_diff>
--- a/inst/extdata/additional_elecdata.xlsx
+++ b/inst/extdata/additional_elecdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Git_Projekte\bundeslaendeR\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au785183\git_projects\bundeslaendeR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576801A1-176B-4427-8502-26E2FFEDFD64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A05F1C1-E7BE-422B-B5B4-7EF69CBADAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1542" uniqueCount="269">
   <si>
     <t>state</t>
   </si>
@@ -706,6 +706,141 @@
   </si>
   <si>
     <t>Wählerliste Klimaliste Hessen</t>
+  </si>
+  <si>
+    <t>SN</t>
+  </si>
+  <si>
+    <t>FW-SN</t>
+  </si>
+  <si>
+    <t>Baisdemokratische Partei Deutschland</t>
+  </si>
+  <si>
+    <t>BD</t>
+  </si>
+  <si>
+    <t>BÜNDNIS DEUTSCHLAND</t>
+  </si>
+  <si>
+    <t>BSW</t>
+  </si>
+  <si>
+    <t>Bündnis Sahra Wagenknecht</t>
+  </si>
+  <si>
+    <t>FS (2021)</t>
+  </si>
+  <si>
+    <t>FREIE SACHSEN</t>
+  </si>
+  <si>
+    <t>WU</t>
+  </si>
+  <si>
+    <t>WerteUnion</t>
+  </si>
+  <si>
+    <t>2024-09-01</t>
+  </si>
+  <si>
+    <t>TH</t>
+  </si>
+  <si>
+    <t>Aktion Partei für Tierschutz</t>
+  </si>
+  <si>
+    <t>ÖDP / Familie ..</t>
+  </si>
+  <si>
+    <t>Ökologisch-Demokratische Partei/Familie, Gerechtigkeit, Umwelt</t>
+  </si>
+  <si>
+    <t>FW-TH</t>
+  </si>
+  <si>
+    <t>FREIE WÄHLER in Thüringen</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>2024-09-22</t>
+  </si>
+  <si>
+    <t>FW-BB</t>
+  </si>
+  <si>
+    <t>PB</t>
+  </si>
+  <si>
+    <t>DritterWeg</t>
+  </si>
+  <si>
+    <t>DLW</t>
+  </si>
+  <si>
+    <t>GRÜNE/B 90</t>
+  </si>
+  <si>
+    <t>BVB / FREIE WÄHLER</t>
+  </si>
+  <si>
+    <t>Plus</t>
+  </si>
+  <si>
+    <t>III. Weg</t>
+  </si>
+  <si>
+    <t>Die Linke</t>
+  </si>
+  <si>
+    <t>Brandenburger Vereinigte Bürgerbewegungen / Freie Wähler</t>
+  </si>
+  <si>
+    <t>Plus Brandenburg</t>
+  </si>
+  <si>
+    <t>Bündnis Sahra Wagenknecht - Vernunft und Gerechtigkeit</t>
+  </si>
+  <si>
+    <t>DER DRITTE WEG</t>
+  </si>
+  <si>
+    <t>Deutsch Land Wirtschaft</t>
+  </si>
+  <si>
+    <t>HH</t>
+  </si>
+  <si>
+    <t>WFG</t>
+  </si>
+  <si>
+    <t>DAVA</t>
+  </si>
+  <si>
+    <t>FW-HH</t>
+  </si>
+  <si>
+    <t>NPD (2023)</t>
+  </si>
+  <si>
+    <t>DieWahl - WFG</t>
+  </si>
+  <si>
+    <t>DAVA-Hamburg</t>
+  </si>
+  <si>
+    <t>Die Wahl für Frieden und soziale Gerechtigkeit</t>
+  </si>
+  <si>
+    <t>Demokratische Allianz für Vielfalt und Aufbruch - Hamburg</t>
+  </si>
+  <si>
+    <t>Nationaldemokratische Partei Deutschlands, Landesverband Hamburg</t>
+  </si>
+  <si>
+    <t>2025-03-02</t>
   </si>
 </sst>
 </file>
@@ -767,7 +902,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1045,14 +1180,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L243"/>
+  <dimension ref="A1:L307"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K148" sqref="K148"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A281" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H303" sqref="H303"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
@@ -10302,6 +10437,2438 @@
         <v>202</v>
       </c>
     </row>
+    <row r="244" spans="1:12">
+      <c r="A244" t="s">
+        <v>224</v>
+      </c>
+      <c r="B244">
+        <v>8</v>
+      </c>
+      <c r="C244">
+        <v>3182683</v>
+      </c>
+      <c r="D244">
+        <v>2367607</v>
+      </c>
+      <c r="E244">
+        <v>2347973</v>
+      </c>
+      <c r="F244">
+        <v>120</v>
+      </c>
+      <c r="G244" t="s">
+        <v>11</v>
+      </c>
+      <c r="H244">
+        <v>749114</v>
+      </c>
+      <c r="I244">
+        <v>41</v>
+      </c>
+      <c r="J244" t="s">
+        <v>11</v>
+      </c>
+      <c r="K244" t="s">
+        <v>46</v>
+      </c>
+      <c r="L244" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="245" spans="1:12">
+      <c r="A245" t="s">
+        <v>224</v>
+      </c>
+      <c r="B245">
+        <v>8</v>
+      </c>
+      <c r="C245">
+        <v>3182683</v>
+      </c>
+      <c r="D245">
+        <v>2367607</v>
+      </c>
+      <c r="E245">
+        <v>2347973</v>
+      </c>
+      <c r="F245">
+        <v>120</v>
+      </c>
+      <c r="G245" t="s">
+        <v>12</v>
+      </c>
+      <c r="H245">
+        <v>719279</v>
+      </c>
+      <c r="I245">
+        <v>40</v>
+      </c>
+      <c r="J245" t="s">
+        <v>12</v>
+      </c>
+      <c r="K245" t="s">
+        <v>47</v>
+      </c>
+      <c r="L245" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="246" spans="1:12">
+      <c r="A246" t="s">
+        <v>224</v>
+      </c>
+      <c r="B246">
+        <v>8</v>
+      </c>
+      <c r="C246">
+        <v>3182683</v>
+      </c>
+      <c r="D246">
+        <v>2367607</v>
+      </c>
+      <c r="E246">
+        <v>2347973</v>
+      </c>
+      <c r="F246">
+        <v>120</v>
+      </c>
+      <c r="G246" t="s">
+        <v>13</v>
+      </c>
+      <c r="H246">
+        <v>104891</v>
+      </c>
+      <c r="I246">
+        <v>6</v>
+      </c>
+      <c r="J246" t="s">
+        <v>35</v>
+      </c>
+      <c r="K246" t="s">
+        <v>35</v>
+      </c>
+      <c r="L246" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="247" spans="1:12">
+      <c r="A247" t="s">
+        <v>224</v>
+      </c>
+      <c r="B247">
+        <v>8</v>
+      </c>
+      <c r="C247">
+        <v>3182683</v>
+      </c>
+      <c r="D247">
+        <v>2367607</v>
+      </c>
+      <c r="E247">
+        <v>2347973</v>
+      </c>
+      <c r="F247">
+        <v>120</v>
+      </c>
+      <c r="G247" t="s">
+        <v>16</v>
+      </c>
+      <c r="H247">
+        <v>119980</v>
+      </c>
+      <c r="I247">
+        <v>7</v>
+      </c>
+      <c r="J247" t="s">
+        <v>36</v>
+      </c>
+      <c r="K247" t="s">
+        <v>50</v>
+      </c>
+      <c r="L247" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="248" spans="1:12">
+      <c r="A248" t="s">
+        <v>224</v>
+      </c>
+      <c r="B248">
+        <v>8</v>
+      </c>
+      <c r="C248">
+        <v>3182683</v>
+      </c>
+      <c r="D248">
+        <v>2367607</v>
+      </c>
+      <c r="E248">
+        <v>2347973</v>
+      </c>
+      <c r="F248">
+        <v>120</v>
+      </c>
+      <c r="G248" t="s">
+        <v>14</v>
+      </c>
+      <c r="H248">
+        <v>172021</v>
+      </c>
+      <c r="I248">
+        <v>10</v>
+      </c>
+      <c r="J248" t="s">
+        <v>14</v>
+      </c>
+      <c r="K248" t="s">
+        <v>48</v>
+      </c>
+      <c r="L248" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="249" spans="1:12">
+      <c r="A249" t="s">
+        <v>224</v>
+      </c>
+      <c r="B249">
+        <v>8</v>
+      </c>
+      <c r="C249">
+        <v>3182683</v>
+      </c>
+      <c r="D249">
+        <v>2367607</v>
+      </c>
+      <c r="E249">
+        <v>2347973</v>
+      </c>
+      <c r="F249">
+        <v>120</v>
+      </c>
+      <c r="G249" t="s">
+        <v>15</v>
+      </c>
+      <c r="H249">
+        <v>20995</v>
+      </c>
+      <c r="I249">
+        <v>0</v>
+      </c>
+      <c r="J249" t="s">
+        <v>15</v>
+      </c>
+      <c r="K249" t="s">
+        <v>49</v>
+      </c>
+      <c r="L249" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="250" spans="1:12">
+      <c r="A250" t="s">
+        <v>224</v>
+      </c>
+      <c r="B250">
+        <v>8</v>
+      </c>
+      <c r="C250">
+        <v>3182683</v>
+      </c>
+      <c r="D250">
+        <v>2367607</v>
+      </c>
+      <c r="E250">
+        <v>2347973</v>
+      </c>
+      <c r="F250">
+        <v>120</v>
+      </c>
+      <c r="G250" t="s">
+        <v>225</v>
+      </c>
+      <c r="H250">
+        <v>53027</v>
+      </c>
+      <c r="I250">
+        <v>1</v>
+      </c>
+      <c r="J250" t="s">
+        <v>37</v>
+      </c>
+      <c r="K250" t="s">
+        <v>37</v>
+      </c>
+      <c r="L250" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="251" spans="1:12">
+      <c r="A251" t="s">
+        <v>224</v>
+      </c>
+      <c r="B251">
+        <v>8</v>
+      </c>
+      <c r="C251">
+        <v>3182683</v>
+      </c>
+      <c r="D251">
+        <v>2367607</v>
+      </c>
+      <c r="E251">
+        <v>2347973</v>
+      </c>
+      <c r="F251">
+        <v>120</v>
+      </c>
+      <c r="G251" t="s">
+        <v>21</v>
+      </c>
+      <c r="H251">
+        <v>19752</v>
+      </c>
+      <c r="I251">
+        <v>0</v>
+      </c>
+      <c r="J251" t="s">
+        <v>40</v>
+      </c>
+      <c r="K251" t="s">
+        <v>191</v>
+      </c>
+      <c r="L251" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="252" spans="1:12">
+      <c r="A252" t="s">
+        <v>224</v>
+      </c>
+      <c r="B252">
+        <v>8</v>
+      </c>
+      <c r="C252">
+        <v>3182683</v>
+      </c>
+      <c r="D252">
+        <v>2367607</v>
+      </c>
+      <c r="E252">
+        <v>2347973</v>
+      </c>
+      <c r="F252">
+        <v>120</v>
+      </c>
+      <c r="G252" t="s">
+        <v>25</v>
+      </c>
+      <c r="H252">
+        <v>6772</v>
+      </c>
+      <c r="I252">
+        <v>0</v>
+      </c>
+      <c r="J252" t="s">
+        <v>43</v>
+      </c>
+      <c r="K252" t="s">
+        <v>56</v>
+      </c>
+      <c r="L252" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="253" spans="1:12">
+      <c r="A253" t="s">
+        <v>224</v>
+      </c>
+      <c r="B253">
+        <v>8</v>
+      </c>
+      <c r="C253">
+        <v>3182683</v>
+      </c>
+      <c r="D253">
+        <v>2367607</v>
+      </c>
+      <c r="E253">
+        <v>2347973</v>
+      </c>
+      <c r="F253">
+        <v>120</v>
+      </c>
+      <c r="G253" t="s">
+        <v>30</v>
+      </c>
+      <c r="H253">
+        <v>1955</v>
+      </c>
+      <c r="I253">
+        <v>0</v>
+      </c>
+      <c r="J253" t="s">
+        <v>30</v>
+      </c>
+      <c r="K253" t="s">
+        <v>60</v>
+      </c>
+      <c r="L253" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="254" spans="1:12">
+      <c r="A254" t="s">
+        <v>224</v>
+      </c>
+      <c r="B254">
+        <v>8</v>
+      </c>
+      <c r="C254">
+        <v>3182683</v>
+      </c>
+      <c r="D254">
+        <v>2367607</v>
+      </c>
+      <c r="E254">
+        <v>2347973</v>
+      </c>
+      <c r="F254">
+        <v>120</v>
+      </c>
+      <c r="G254" t="s">
+        <v>66</v>
+      </c>
+      <c r="H254">
+        <v>1582</v>
+      </c>
+      <c r="I254">
+        <v>0</v>
+      </c>
+      <c r="J254" t="s">
+        <v>82</v>
+      </c>
+      <c r="K254" t="s">
+        <v>97</v>
+      </c>
+      <c r="L254" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="255" spans="1:12">
+      <c r="A255" t="s">
+        <v>224</v>
+      </c>
+      <c r="B255">
+        <v>8</v>
+      </c>
+      <c r="C255">
+        <v>3182683</v>
+      </c>
+      <c r="D255">
+        <v>2367607</v>
+      </c>
+      <c r="E255">
+        <v>2347973</v>
+      </c>
+      <c r="F255">
+        <v>120</v>
+      </c>
+      <c r="G255" t="s">
+        <v>22</v>
+      </c>
+      <c r="H255">
+        <v>23606</v>
+      </c>
+      <c r="I255">
+        <v>0</v>
+      </c>
+      <c r="J255" t="s">
+        <v>41</v>
+      </c>
+      <c r="K255" t="s">
+        <v>53</v>
+      </c>
+      <c r="L255" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="256" spans="1:12">
+      <c r="A256" t="s">
+        <v>224</v>
+      </c>
+      <c r="B256">
+        <v>8</v>
+      </c>
+      <c r="C256">
+        <v>3182683</v>
+      </c>
+      <c r="D256">
+        <v>2367607</v>
+      </c>
+      <c r="E256">
+        <v>2347973</v>
+      </c>
+      <c r="F256">
+        <v>120</v>
+      </c>
+      <c r="G256" t="s">
+        <v>18</v>
+      </c>
+      <c r="H256">
+        <v>4486</v>
+      </c>
+      <c r="I256">
+        <v>0</v>
+      </c>
+      <c r="J256" t="s">
+        <v>18</v>
+      </c>
+      <c r="K256" t="s">
+        <v>226</v>
+      </c>
+      <c r="L256" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="257" spans="1:12">
+      <c r="A257" t="s">
+        <v>224</v>
+      </c>
+      <c r="B257">
+        <v>8</v>
+      </c>
+      <c r="C257">
+        <v>3182683</v>
+      </c>
+      <c r="D257">
+        <v>2367607</v>
+      </c>
+      <c r="E257">
+        <v>2347973</v>
+      </c>
+      <c r="F257">
+        <v>120</v>
+      </c>
+      <c r="G257" t="s">
+        <v>113</v>
+      </c>
+      <c r="H257">
+        <v>4370</v>
+      </c>
+      <c r="I257">
+        <v>0</v>
+      </c>
+      <c r="J257" t="s">
+        <v>118</v>
+      </c>
+      <c r="K257" t="s">
+        <v>122</v>
+      </c>
+      <c r="L257" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="258" spans="1:12">
+      <c r="A258" t="s">
+        <v>224</v>
+      </c>
+      <c r="B258">
+        <v>8</v>
+      </c>
+      <c r="C258">
+        <v>3182683</v>
+      </c>
+      <c r="D258">
+        <v>2367607</v>
+      </c>
+      <c r="E258">
+        <v>2347973</v>
+      </c>
+      <c r="F258">
+        <v>120</v>
+      </c>
+      <c r="G258" t="s">
+        <v>227</v>
+      </c>
+      <c r="H258">
+        <v>6718</v>
+      </c>
+      <c r="I258">
+        <v>0</v>
+      </c>
+      <c r="J258" t="s">
+        <v>228</v>
+      </c>
+      <c r="K258" t="s">
+        <v>228</v>
+      </c>
+      <c r="L258" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="259" spans="1:12">
+      <c r="A259" t="s">
+        <v>224</v>
+      </c>
+      <c r="B259">
+        <v>8</v>
+      </c>
+      <c r="C259">
+        <v>3182683</v>
+      </c>
+      <c r="D259">
+        <v>2367607</v>
+      </c>
+      <c r="E259">
+        <v>2347973</v>
+      </c>
+      <c r="F259">
+        <v>120</v>
+      </c>
+      <c r="G259" t="s">
+        <v>229</v>
+      </c>
+      <c r="H259">
+        <v>277568</v>
+      </c>
+      <c r="I259">
+        <v>15</v>
+      </c>
+      <c r="J259" t="s">
+        <v>229</v>
+      </c>
+      <c r="K259" t="s">
+        <v>230</v>
+      </c>
+      <c r="L259" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="260" spans="1:12">
+      <c r="A260" t="s">
+        <v>224</v>
+      </c>
+      <c r="B260">
+        <v>8</v>
+      </c>
+      <c r="C260">
+        <v>3182683</v>
+      </c>
+      <c r="D260">
+        <v>2367607</v>
+      </c>
+      <c r="E260">
+        <v>2347973</v>
+      </c>
+      <c r="F260">
+        <v>120</v>
+      </c>
+      <c r="G260" t="s">
+        <v>231</v>
+      </c>
+      <c r="H260">
+        <v>52100</v>
+      </c>
+      <c r="I260">
+        <v>0</v>
+      </c>
+      <c r="J260" t="s">
+        <v>232</v>
+      </c>
+      <c r="K260" t="s">
+        <v>232</v>
+      </c>
+      <c r="L260" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="261" spans="1:12">
+      <c r="A261" t="s">
+        <v>224</v>
+      </c>
+      <c r="B261">
+        <v>8</v>
+      </c>
+      <c r="C261">
+        <v>3182683</v>
+      </c>
+      <c r="D261">
+        <v>2367607</v>
+      </c>
+      <c r="E261">
+        <v>2347973</v>
+      </c>
+      <c r="F261">
+        <v>120</v>
+      </c>
+      <c r="G261" t="s">
+        <v>206</v>
+      </c>
+      <c r="H261">
+        <v>3283</v>
+      </c>
+      <c r="I261">
+        <v>0</v>
+      </c>
+      <c r="J261" t="s">
+        <v>207</v>
+      </c>
+      <c r="K261" t="s">
+        <v>220</v>
+      </c>
+      <c r="L261" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="262" spans="1:12">
+      <c r="A262" t="s">
+        <v>224</v>
+      </c>
+      <c r="B262">
+        <v>8</v>
+      </c>
+      <c r="C262">
+        <v>3182683</v>
+      </c>
+      <c r="D262">
+        <v>2367607</v>
+      </c>
+      <c r="E262">
+        <v>2347973</v>
+      </c>
+      <c r="F262">
+        <v>120</v>
+      </c>
+      <c r="G262" t="s">
+        <v>233</v>
+      </c>
+      <c r="H262">
+        <v>6474</v>
+      </c>
+      <c r="I262">
+        <v>0</v>
+      </c>
+      <c r="J262" t="s">
+        <v>233</v>
+      </c>
+      <c r="K262" t="s">
+        <v>234</v>
+      </c>
+      <c r="L262" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="263" spans="1:12">
+      <c r="A263" t="s">
+        <v>236</v>
+      </c>
+      <c r="B263">
+        <v>8</v>
+      </c>
+      <c r="C263">
+        <v>1655670</v>
+      </c>
+      <c r="D263">
+        <v>1218089</v>
+      </c>
+      <c r="E263">
+        <v>1207883</v>
+      </c>
+      <c r="F263">
+        <v>88</v>
+      </c>
+      <c r="G263" t="s">
+        <v>13</v>
+      </c>
+      <c r="H263">
+        <v>157689</v>
+      </c>
+      <c r="I263">
+        <v>12</v>
+      </c>
+      <c r="J263" t="s">
+        <v>35</v>
+      </c>
+      <c r="K263" t="s">
+        <v>35</v>
+      </c>
+      <c r="L263" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="264" spans="1:12">
+      <c r="A264" t="s">
+        <v>236</v>
+      </c>
+      <c r="B264">
+        <v>8</v>
+      </c>
+      <c r="C264">
+        <v>1655670</v>
+      </c>
+      <c r="D264">
+        <v>1218089</v>
+      </c>
+      <c r="E264">
+        <v>1207883</v>
+      </c>
+      <c r="F264">
+        <v>88</v>
+      </c>
+      <c r="G264" t="s">
+        <v>12</v>
+      </c>
+      <c r="H264">
+        <v>396711</v>
+      </c>
+      <c r="I264">
+        <v>32</v>
+      </c>
+      <c r="J264" t="s">
+        <v>12</v>
+      </c>
+      <c r="K264" t="s">
+        <v>47</v>
+      </c>
+      <c r="L264" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="265" spans="1:12">
+      <c r="A265" t="s">
+        <v>236</v>
+      </c>
+      <c r="B265">
+        <v>8</v>
+      </c>
+      <c r="C265">
+        <v>1655670</v>
+      </c>
+      <c r="D265">
+        <v>1218089</v>
+      </c>
+      <c r="E265">
+        <v>1207883</v>
+      </c>
+      <c r="F265">
+        <v>88</v>
+      </c>
+      <c r="G265" t="s">
+        <v>11</v>
+      </c>
+      <c r="H265">
+        <v>285097</v>
+      </c>
+      <c r="I265">
+        <v>23</v>
+      </c>
+      <c r="J265" t="s">
+        <v>11</v>
+      </c>
+      <c r="K265" t="s">
+        <v>46</v>
+      </c>
+      <c r="L265" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="266" spans="1:12">
+      <c r="A266" t="s">
+        <v>236</v>
+      </c>
+      <c r="B266">
+        <v>8</v>
+      </c>
+      <c r="C266">
+        <v>1655670</v>
+      </c>
+      <c r="D266">
+        <v>1218089</v>
+      </c>
+      <c r="E266">
+        <v>1207883</v>
+      </c>
+      <c r="F266">
+        <v>88</v>
+      </c>
+      <c r="G266" t="s">
+        <v>14</v>
+      </c>
+      <c r="H266">
+        <v>73126</v>
+      </c>
+      <c r="I266">
+        <v>6</v>
+      </c>
+      <c r="J266" t="s">
+        <v>14</v>
+      </c>
+      <c r="K266" t="s">
+        <v>48</v>
+      </c>
+      <c r="L266" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="267" spans="1:12">
+      <c r="A267" t="s">
+        <v>236</v>
+      </c>
+      <c r="B267">
+        <v>8</v>
+      </c>
+      <c r="C267">
+        <v>1655670</v>
+      </c>
+      <c r="D267">
+        <v>1218089</v>
+      </c>
+      <c r="E267">
+        <v>1207883</v>
+      </c>
+      <c r="F267">
+        <v>88</v>
+      </c>
+      <c r="G267" t="s">
+        <v>16</v>
+      </c>
+      <c r="H267">
+        <v>38275</v>
+      </c>
+      <c r="I267">
+        <v>0</v>
+      </c>
+      <c r="J267" t="s">
+        <v>36</v>
+      </c>
+      <c r="K267" t="s">
+        <v>50</v>
+      </c>
+      <c r="L267" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="268" spans="1:12">
+      <c r="A268" t="s">
+        <v>236</v>
+      </c>
+      <c r="B268">
+        <v>8</v>
+      </c>
+      <c r="C268">
+        <v>1655670</v>
+      </c>
+      <c r="D268">
+        <v>1218089</v>
+      </c>
+      <c r="E268">
+        <v>1207883</v>
+      </c>
+      <c r="F268">
+        <v>88</v>
+      </c>
+      <c r="G268" t="s">
+        <v>15</v>
+      </c>
+      <c r="H268">
+        <v>13591</v>
+      </c>
+      <c r="I268">
+        <v>0</v>
+      </c>
+      <c r="J268" t="s">
+        <v>15</v>
+      </c>
+      <c r="K268" t="s">
+        <v>49</v>
+      </c>
+      <c r="L268" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="269" spans="1:12">
+      <c r="A269" t="s">
+        <v>236</v>
+      </c>
+      <c r="B269">
+        <v>8</v>
+      </c>
+      <c r="C269">
+        <v>1655670</v>
+      </c>
+      <c r="D269">
+        <v>1218089</v>
+      </c>
+      <c r="E269">
+        <v>1207883</v>
+      </c>
+      <c r="F269">
+        <v>88</v>
+      </c>
+      <c r="G269" t="s">
+        <v>22</v>
+      </c>
+      <c r="H269">
+        <v>12112</v>
+      </c>
+      <c r="I269">
+        <v>0</v>
+      </c>
+      <c r="J269" t="s">
+        <v>41</v>
+      </c>
+      <c r="K269" t="s">
+        <v>237</v>
+      </c>
+      <c r="L269" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="270" spans="1:12">
+      <c r="A270" t="s">
+        <v>236</v>
+      </c>
+      <c r="B270">
+        <v>8</v>
+      </c>
+      <c r="C270">
+        <v>1655670</v>
+      </c>
+      <c r="D270">
+        <v>1218089</v>
+      </c>
+      <c r="E270">
+        <v>1207883</v>
+      </c>
+      <c r="F270">
+        <v>88</v>
+      </c>
+      <c r="G270" t="s">
+        <v>30</v>
+      </c>
+      <c r="H270">
+        <v>2389</v>
+      </c>
+      <c r="I270">
+        <v>0</v>
+      </c>
+      <c r="J270" t="s">
+        <v>238</v>
+      </c>
+      <c r="K270" t="s">
+        <v>239</v>
+      </c>
+      <c r="L270" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="271" spans="1:12">
+      <c r="A271" t="s">
+        <v>236</v>
+      </c>
+      <c r="B271">
+        <v>8</v>
+      </c>
+      <c r="C271">
+        <v>1655670</v>
+      </c>
+      <c r="D271">
+        <v>1218089</v>
+      </c>
+      <c r="E271">
+        <v>1207883</v>
+      </c>
+      <c r="F271">
+        <v>88</v>
+      </c>
+      <c r="G271" t="s">
+        <v>147</v>
+      </c>
+      <c r="H271">
+        <v>1327</v>
+      </c>
+      <c r="I271">
+        <v>0</v>
+      </c>
+      <c r="J271" t="s">
+        <v>147</v>
+      </c>
+      <c r="K271" t="s">
+        <v>154</v>
+      </c>
+      <c r="L271" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="272" spans="1:12">
+      <c r="A272" t="s">
+        <v>236</v>
+      </c>
+      <c r="B272">
+        <v>8</v>
+      </c>
+      <c r="C272">
+        <v>1655670</v>
+      </c>
+      <c r="D272">
+        <v>1218089</v>
+      </c>
+      <c r="E272">
+        <v>1207883</v>
+      </c>
+      <c r="F272">
+        <v>88</v>
+      </c>
+      <c r="G272" t="s">
+        <v>227</v>
+      </c>
+      <c r="H272">
+        <v>5309</v>
+      </c>
+      <c r="I272">
+        <v>0</v>
+      </c>
+      <c r="J272" t="s">
+        <v>228</v>
+      </c>
+      <c r="K272" t="s">
+        <v>228</v>
+      </c>
+      <c r="L272" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="273" spans="1:12">
+      <c r="A273" t="s">
+        <v>236</v>
+      </c>
+      <c r="B273">
+        <v>8</v>
+      </c>
+      <c r="C273">
+        <v>1655670</v>
+      </c>
+      <c r="D273">
+        <v>1218089</v>
+      </c>
+      <c r="E273">
+        <v>1207883</v>
+      </c>
+      <c r="F273">
+        <v>88</v>
+      </c>
+      <c r="G273" t="s">
+        <v>229</v>
+      </c>
+      <c r="H273">
+        <v>190664</v>
+      </c>
+      <c r="I273">
+        <v>15</v>
+      </c>
+      <c r="J273" t="s">
+        <v>229</v>
+      </c>
+      <c r="K273" t="s">
+        <v>230</v>
+      </c>
+      <c r="L273" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="274" spans="1:12">
+      <c r="A274" t="s">
+        <v>236</v>
+      </c>
+      <c r="B274">
+        <v>8</v>
+      </c>
+      <c r="C274">
+        <v>1655670</v>
+      </c>
+      <c r="D274">
+        <v>1218089</v>
+      </c>
+      <c r="E274">
+        <v>1207883</v>
+      </c>
+      <c r="F274">
+        <v>88</v>
+      </c>
+      <c r="G274" t="s">
+        <v>132</v>
+      </c>
+      <c r="H274">
+        <v>5709</v>
+      </c>
+      <c r="I274">
+        <v>0</v>
+      </c>
+      <c r="J274" t="s">
+        <v>133</v>
+      </c>
+      <c r="K274" t="s">
+        <v>134</v>
+      </c>
+      <c r="L274" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="275" spans="1:12">
+      <c r="A275" t="s">
+        <v>236</v>
+      </c>
+      <c r="B275">
+        <v>8</v>
+      </c>
+      <c r="C275">
+        <v>1655670</v>
+      </c>
+      <c r="D275">
+        <v>1218089</v>
+      </c>
+      <c r="E275">
+        <v>1207883</v>
+      </c>
+      <c r="F275">
+        <v>88</v>
+      </c>
+      <c r="G275" t="s">
+        <v>240</v>
+      </c>
+      <c r="H275">
+        <v>15385</v>
+      </c>
+      <c r="I275">
+        <v>0</v>
+      </c>
+      <c r="J275" t="s">
+        <v>37</v>
+      </c>
+      <c r="K275" t="s">
+        <v>241</v>
+      </c>
+      <c r="L275" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="276" spans="1:12">
+      <c r="A276" t="s">
+        <v>236</v>
+      </c>
+      <c r="B276">
+        <v>8</v>
+      </c>
+      <c r="C276">
+        <v>1655670</v>
+      </c>
+      <c r="D276">
+        <v>1218089</v>
+      </c>
+      <c r="E276">
+        <v>1207883</v>
+      </c>
+      <c r="F276">
+        <v>88</v>
+      </c>
+      <c r="G276" t="s">
+        <v>233</v>
+      </c>
+      <c r="H276">
+        <v>6778</v>
+      </c>
+      <c r="I276">
+        <v>0</v>
+      </c>
+      <c r="J276" t="s">
+        <v>233</v>
+      </c>
+      <c r="K276" t="s">
+        <v>234</v>
+      </c>
+      <c r="L276" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="277" spans="1:12">
+      <c r="A277" t="s">
+        <v>236</v>
+      </c>
+      <c r="B277">
+        <v>8</v>
+      </c>
+      <c r="C277">
+        <v>1655670</v>
+      </c>
+      <c r="D277">
+        <v>1218089</v>
+      </c>
+      <c r="E277">
+        <v>1207883</v>
+      </c>
+      <c r="F277">
+        <v>88</v>
+      </c>
+      <c r="G277" t="s">
+        <v>25</v>
+      </c>
+      <c r="H277">
+        <v>3721</v>
+      </c>
+      <c r="I277">
+        <v>0</v>
+      </c>
+      <c r="J277" t="s">
+        <v>43</v>
+      </c>
+      <c r="K277" t="s">
+        <v>56</v>
+      </c>
+      <c r="L277" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="278" spans="1:12">
+      <c r="A278" t="s">
+        <v>242</v>
+      </c>
+      <c r="B278">
+        <v>8</v>
+      </c>
+      <c r="C278">
+        <v>2076920</v>
+      </c>
+      <c r="D278">
+        <v>1513975</v>
+      </c>
+      <c r="E278">
+        <v>1501619</v>
+      </c>
+      <c r="F278">
+        <v>88</v>
+      </c>
+      <c r="G278" t="s">
+        <v>14</v>
+      </c>
+      <c r="H278">
+        <v>463800</v>
+      </c>
+      <c r="I278">
+        <v>32</v>
+      </c>
+      <c r="J278" t="s">
+        <v>14</v>
+      </c>
+      <c r="K278" t="s">
+        <v>48</v>
+      </c>
+      <c r="L278" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="279" spans="1:12">
+      <c r="A279" t="s">
+        <v>242</v>
+      </c>
+      <c r="B279">
+        <v>8</v>
+      </c>
+      <c r="C279">
+        <v>2076920</v>
+      </c>
+      <c r="D279">
+        <v>1513975</v>
+      </c>
+      <c r="E279">
+        <v>1501619</v>
+      </c>
+      <c r="F279">
+        <v>88</v>
+      </c>
+      <c r="G279" t="s">
+        <v>12</v>
+      </c>
+      <c r="H279">
+        <v>438904</v>
+      </c>
+      <c r="I279">
+        <v>30</v>
+      </c>
+      <c r="J279" t="s">
+        <v>12</v>
+      </c>
+      <c r="K279" t="s">
+        <v>47</v>
+      </c>
+      <c r="L279" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="280" spans="1:12">
+      <c r="A280" t="s">
+        <v>242</v>
+      </c>
+      <c r="B280">
+        <v>8</v>
+      </c>
+      <c r="C280">
+        <v>2076920</v>
+      </c>
+      <c r="D280">
+        <v>1513975</v>
+      </c>
+      <c r="E280">
+        <v>1501619</v>
+      </c>
+      <c r="F280">
+        <v>88</v>
+      </c>
+      <c r="G280" t="s">
+        <v>11</v>
+      </c>
+      <c r="H280">
+        <v>181716</v>
+      </c>
+      <c r="I280">
+        <v>12</v>
+      </c>
+      <c r="J280" t="s">
+        <v>11</v>
+      </c>
+      <c r="K280" t="s">
+        <v>46</v>
+      </c>
+      <c r="L280" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="281" spans="1:12">
+      <c r="A281" t="s">
+        <v>242</v>
+      </c>
+      <c r="B281">
+        <v>8</v>
+      </c>
+      <c r="C281">
+        <v>2076920</v>
+      </c>
+      <c r="D281">
+        <v>1513975</v>
+      </c>
+      <c r="E281">
+        <v>1501619</v>
+      </c>
+      <c r="F281">
+        <v>88</v>
+      </c>
+      <c r="G281" t="s">
+        <v>16</v>
+      </c>
+      <c r="H281">
+        <v>62057</v>
+      </c>
+      <c r="I281">
+        <v>0</v>
+      </c>
+      <c r="J281" t="s">
+        <v>248</v>
+      </c>
+      <c r="K281" t="s">
+        <v>50</v>
+      </c>
+      <c r="L281" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="282" spans="1:12">
+      <c r="A282" t="s">
+        <v>242</v>
+      </c>
+      <c r="B282">
+        <v>8</v>
+      </c>
+      <c r="C282">
+        <v>2076920</v>
+      </c>
+      <c r="D282">
+        <v>1513975</v>
+      </c>
+      <c r="E282">
+        <v>1501619</v>
+      </c>
+      <c r="F282">
+        <v>88</v>
+      </c>
+      <c r="G282" t="s">
+        <v>13</v>
+      </c>
+      <c r="H282">
+        <v>44706</v>
+      </c>
+      <c r="I282">
+        <v>0</v>
+      </c>
+      <c r="J282" t="s">
+        <v>35</v>
+      </c>
+      <c r="K282" t="s">
+        <v>35</v>
+      </c>
+      <c r="L282" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="283" spans="1:12">
+      <c r="A283" t="s">
+        <v>242</v>
+      </c>
+      <c r="B283">
+        <v>8</v>
+      </c>
+      <c r="C283">
+        <v>2076920</v>
+      </c>
+      <c r="D283">
+        <v>1513975</v>
+      </c>
+      <c r="E283">
+        <v>1501619</v>
+      </c>
+      <c r="F283">
+        <v>88</v>
+      </c>
+      <c r="G283" t="s">
+        <v>244</v>
+      </c>
+      <c r="H283">
+        <v>38573</v>
+      </c>
+      <c r="I283">
+        <v>0</v>
+      </c>
+      <c r="J283" t="s">
+        <v>249</v>
+      </c>
+      <c r="K283" t="s">
+        <v>253</v>
+      </c>
+      <c r="L283" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="284" spans="1:12">
+      <c r="A284" t="s">
+        <v>242</v>
+      </c>
+      <c r="B284">
+        <v>8</v>
+      </c>
+      <c r="C284">
+        <v>2076920</v>
+      </c>
+      <c r="D284">
+        <v>1513975</v>
+      </c>
+      <c r="E284">
+        <v>1501619</v>
+      </c>
+      <c r="F284">
+        <v>88</v>
+      </c>
+      <c r="G284" t="s">
+        <v>15</v>
+      </c>
+      <c r="H284">
+        <v>12475</v>
+      </c>
+      <c r="I284">
+        <v>0</v>
+      </c>
+      <c r="J284" t="s">
+        <v>15</v>
+      </c>
+      <c r="K284" t="s">
+        <v>49</v>
+      </c>
+      <c r="L284" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="285" spans="1:12">
+      <c r="A285" t="s">
+        <v>242</v>
+      </c>
+      <c r="B285">
+        <v>8</v>
+      </c>
+      <c r="C285">
+        <v>2076920</v>
+      </c>
+      <c r="D285">
+        <v>1513975</v>
+      </c>
+      <c r="E285">
+        <v>1501619</v>
+      </c>
+      <c r="F285">
+        <v>88</v>
+      </c>
+      <c r="G285" t="s">
+        <v>19</v>
+      </c>
+      <c r="H285">
+        <v>30041</v>
+      </c>
+      <c r="I285">
+        <v>0</v>
+      </c>
+      <c r="J285" t="s">
+        <v>38</v>
+      </c>
+      <c r="K285" t="s">
+        <v>52</v>
+      </c>
+      <c r="L285" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="286" spans="1:12">
+      <c r="A286" t="s">
+        <v>242</v>
+      </c>
+      <c r="B286">
+        <v>8</v>
+      </c>
+      <c r="C286">
+        <v>2076920</v>
+      </c>
+      <c r="D286">
+        <v>1513975</v>
+      </c>
+      <c r="E286">
+        <v>1501619</v>
+      </c>
+      <c r="F286">
+        <v>88</v>
+      </c>
+      <c r="G286" t="s">
+        <v>245</v>
+      </c>
+      <c r="H286">
+        <v>13584</v>
+      </c>
+      <c r="I286">
+        <v>0</v>
+      </c>
+      <c r="J286" t="s">
+        <v>250</v>
+      </c>
+      <c r="K286" t="s">
+        <v>254</v>
+      </c>
+      <c r="L286" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="287" spans="1:12">
+      <c r="A287" t="s">
+        <v>242</v>
+      </c>
+      <c r="B287">
+        <v>8</v>
+      </c>
+      <c r="C287">
+        <v>2076920</v>
+      </c>
+      <c r="D287">
+        <v>1513975</v>
+      </c>
+      <c r="E287">
+        <v>1501619</v>
+      </c>
+      <c r="F287">
+        <v>88</v>
+      </c>
+      <c r="G287" t="s">
+        <v>229</v>
+      </c>
+      <c r="H287">
+        <v>202421</v>
+      </c>
+      <c r="I287">
+        <v>14</v>
+      </c>
+      <c r="J287" t="s">
+        <v>229</v>
+      </c>
+      <c r="K287" t="s">
+        <v>255</v>
+      </c>
+      <c r="L287" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="288" spans="1:12">
+      <c r="A288" t="s">
+        <v>242</v>
+      </c>
+      <c r="B288">
+        <v>8</v>
+      </c>
+      <c r="C288">
+        <v>2076920</v>
+      </c>
+      <c r="D288">
+        <v>1513975</v>
+      </c>
+      <c r="E288">
+        <v>1501619</v>
+      </c>
+      <c r="F288">
+        <v>88</v>
+      </c>
+      <c r="G288" t="s">
+        <v>246</v>
+      </c>
+      <c r="H288">
+        <v>1810</v>
+      </c>
+      <c r="I288">
+        <v>0</v>
+      </c>
+      <c r="J288" t="s">
+        <v>251</v>
+      </c>
+      <c r="K288" t="s">
+        <v>256</v>
+      </c>
+      <c r="L288" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="289" spans="1:12">
+      <c r="A289" t="s">
+        <v>242</v>
+      </c>
+      <c r="B289">
+        <v>8</v>
+      </c>
+      <c r="C289">
+        <v>2076920</v>
+      </c>
+      <c r="D289">
+        <v>1513975</v>
+      </c>
+      <c r="E289">
+        <v>1501619</v>
+      </c>
+      <c r="F289">
+        <v>88</v>
+      </c>
+      <c r="G289" t="s">
+        <v>64</v>
+      </c>
+      <c r="H289">
+        <v>1021</v>
+      </c>
+      <c r="I289">
+        <v>0</v>
+      </c>
+      <c r="J289" t="s">
+        <v>64</v>
+      </c>
+      <c r="K289" t="s">
+        <v>95</v>
+      </c>
+      <c r="L289" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="290" spans="1:12">
+      <c r="A290" t="s">
+        <v>242</v>
+      </c>
+      <c r="B290">
+        <v>8</v>
+      </c>
+      <c r="C290">
+        <v>2076920</v>
+      </c>
+      <c r="D290">
+        <v>1513975</v>
+      </c>
+      <c r="E290">
+        <v>1501619</v>
+      </c>
+      <c r="F290">
+        <v>88</v>
+      </c>
+      <c r="G290" t="s">
+        <v>247</v>
+      </c>
+      <c r="H290">
+        <v>6633</v>
+      </c>
+      <c r="I290">
+        <v>0</v>
+      </c>
+      <c r="J290" t="s">
+        <v>247</v>
+      </c>
+      <c r="K290" t="s">
+        <v>257</v>
+      </c>
+      <c r="L290" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="291" spans="1:12">
+      <c r="A291" t="s">
+        <v>242</v>
+      </c>
+      <c r="B291">
+        <v>8</v>
+      </c>
+      <c r="C291">
+        <v>2076920</v>
+      </c>
+      <c r="D291">
+        <v>1513975</v>
+      </c>
+      <c r="E291">
+        <v>1501619</v>
+      </c>
+      <c r="F291">
+        <v>88</v>
+      </c>
+      <c r="G291" t="s">
+        <v>233</v>
+      </c>
+      <c r="H291">
+        <v>3878</v>
+      </c>
+      <c r="I291">
+        <v>0</v>
+      </c>
+      <c r="J291" t="s">
+        <v>233</v>
+      </c>
+      <c r="K291" t="s">
+        <v>234</v>
+      </c>
+      <c r="L291" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="292" spans="1:12">
+      <c r="A292" t="s">
+        <v>258</v>
+      </c>
+      <c r="B292">
+        <v>23</v>
+      </c>
+      <c r="C292">
+        <v>1313043</v>
+      </c>
+      <c r="D292">
+        <v>887742</v>
+      </c>
+      <c r="E292">
+        <v>4371246</v>
+      </c>
+      <c r="F292">
+        <v>121</v>
+      </c>
+      <c r="G292" t="s">
+        <v>14</v>
+      </c>
+      <c r="H292">
+        <v>1465023</v>
+      </c>
+      <c r="I292">
+        <v>45</v>
+      </c>
+      <c r="J292" t="s">
+        <v>14</v>
+      </c>
+      <c r="K292" t="s">
+        <v>48</v>
+      </c>
+      <c r="L292" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="293" spans="1:12">
+      <c r="A293" t="s">
+        <v>258</v>
+      </c>
+      <c r="B293">
+        <v>23</v>
+      </c>
+      <c r="C293">
+        <v>1313043</v>
+      </c>
+      <c r="D293">
+        <v>887742</v>
+      </c>
+      <c r="E293">
+        <v>4371246</v>
+      </c>
+      <c r="F293">
+        <v>121</v>
+      </c>
+      <c r="G293" t="s">
+        <v>11</v>
+      </c>
+      <c r="H293">
+        <v>865713</v>
+      </c>
+      <c r="I293">
+        <v>26</v>
+      </c>
+      <c r="J293" t="s">
+        <v>11</v>
+      </c>
+      <c r="K293" t="s">
+        <v>46</v>
+      </c>
+      <c r="L293" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="294" spans="1:12">
+      <c r="A294" t="s">
+        <v>258</v>
+      </c>
+      <c r="B294">
+        <v>23</v>
+      </c>
+      <c r="C294">
+        <v>1313043</v>
+      </c>
+      <c r="D294">
+        <v>887742</v>
+      </c>
+      <c r="E294">
+        <v>4371246</v>
+      </c>
+      <c r="F294">
+        <v>121</v>
+      </c>
+      <c r="G294" t="s">
+        <v>15</v>
+      </c>
+      <c r="H294">
+        <v>100657</v>
+      </c>
+      <c r="I294">
+        <v>0</v>
+      </c>
+      <c r="J294" t="s">
+        <v>15</v>
+      </c>
+      <c r="K294" t="s">
+        <v>49</v>
+      </c>
+      <c r="L294" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="295" spans="1:12">
+      <c r="A295" t="s">
+        <v>258</v>
+      </c>
+      <c r="B295">
+        <v>23</v>
+      </c>
+      <c r="C295">
+        <v>1313043</v>
+      </c>
+      <c r="D295">
+        <v>887742</v>
+      </c>
+      <c r="E295">
+        <v>4371246</v>
+      </c>
+      <c r="F295">
+        <v>121</v>
+      </c>
+      <c r="G295" t="s">
+        <v>16</v>
+      </c>
+      <c r="H295">
+        <v>806660</v>
+      </c>
+      <c r="I295">
+        <v>25</v>
+      </c>
+      <c r="J295" t="s">
+        <v>36</v>
+      </c>
+      <c r="K295" t="s">
+        <v>50</v>
+      </c>
+      <c r="L295" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="296" spans="1:12">
+      <c r="A296" t="s">
+        <v>258</v>
+      </c>
+      <c r="B296">
+        <v>23</v>
+      </c>
+      <c r="C296">
+        <v>1313043</v>
+      </c>
+      <c r="D296">
+        <v>887742</v>
+      </c>
+      <c r="E296">
+        <v>4371246</v>
+      </c>
+      <c r="F296">
+        <v>121</v>
+      </c>
+      <c r="G296" t="s">
+        <v>79</v>
+      </c>
+      <c r="H296">
+        <v>141661</v>
+      </c>
+      <c r="I296">
+        <v>0</v>
+      </c>
+      <c r="J296" t="s">
+        <v>79</v>
+      </c>
+      <c r="K296" t="s">
+        <v>109</v>
+      </c>
+      <c r="L296" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="297" spans="1:12">
+      <c r="A297" t="s">
+        <v>258</v>
+      </c>
+      <c r="B297">
+        <v>23</v>
+      </c>
+      <c r="C297">
+        <v>1313043</v>
+      </c>
+      <c r="D297">
+        <v>887742</v>
+      </c>
+      <c r="E297">
+        <v>4371246</v>
+      </c>
+      <c r="F297">
+        <v>121</v>
+      </c>
+      <c r="G297" t="s">
+        <v>13</v>
+      </c>
+      <c r="H297">
+        <v>488463</v>
+      </c>
+      <c r="I297">
+        <v>15</v>
+      </c>
+      <c r="J297" t="s">
+        <v>252</v>
+      </c>
+      <c r="K297" t="s">
+        <v>252</v>
+      </c>
+      <c r="L297" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="298" spans="1:12">
+      <c r="A298" t="s">
+        <v>258</v>
+      </c>
+      <c r="B298">
+        <v>23</v>
+      </c>
+      <c r="C298">
+        <v>1313043</v>
+      </c>
+      <c r="D298">
+        <v>887742</v>
+      </c>
+      <c r="E298">
+        <v>4371246</v>
+      </c>
+      <c r="F298">
+        <v>121</v>
+      </c>
+      <c r="G298" t="s">
+        <v>12</v>
+      </c>
+      <c r="H298">
+        <v>329651</v>
+      </c>
+      <c r="I298">
+        <v>10</v>
+      </c>
+      <c r="J298" t="s">
+        <v>12</v>
+      </c>
+      <c r="K298" t="s">
+        <v>47</v>
+      </c>
+      <c r="L298" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="299" spans="1:12">
+      <c r="A299" t="s">
+        <v>258</v>
+      </c>
+      <c r="B299">
+        <v>23</v>
+      </c>
+      <c r="C299">
+        <v>1313043</v>
+      </c>
+      <c r="D299">
+        <v>887742</v>
+      </c>
+      <c r="E299">
+        <v>4371246</v>
+      </c>
+      <c r="F299">
+        <v>121</v>
+      </c>
+      <c r="G299" t="s">
+        <v>259</v>
+      </c>
+      <c r="H299">
+        <v>7259</v>
+      </c>
+      <c r="I299">
+        <v>0</v>
+      </c>
+      <c r="J299" t="s">
+        <v>263</v>
+      </c>
+      <c r="K299" t="s">
+        <v>265</v>
+      </c>
+      <c r="L299" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="300" spans="1:12">
+      <c r="A300" t="s">
+        <v>258</v>
+      </c>
+      <c r="B300">
+        <v>23</v>
+      </c>
+      <c r="C300">
+        <v>1313043</v>
+      </c>
+      <c r="D300">
+        <v>887742</v>
+      </c>
+      <c r="E300">
+        <v>4371246</v>
+      </c>
+      <c r="F300">
+        <v>121</v>
+      </c>
+      <c r="G300" t="s">
+        <v>260</v>
+      </c>
+      <c r="H300">
+        <v>25250</v>
+      </c>
+      <c r="I300">
+        <v>0</v>
+      </c>
+      <c r="J300" t="s">
+        <v>264</v>
+      </c>
+      <c r="K300" t="s">
+        <v>266</v>
+      </c>
+      <c r="L300" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="301" spans="1:12">
+      <c r="A301" t="s">
+        <v>258</v>
+      </c>
+      <c r="B301">
+        <v>23</v>
+      </c>
+      <c r="C301">
+        <v>1313043</v>
+      </c>
+      <c r="D301">
+        <v>887742</v>
+      </c>
+      <c r="E301">
+        <v>4371246</v>
+      </c>
+      <c r="F301">
+        <v>121</v>
+      </c>
+      <c r="G301" t="s">
+        <v>261</v>
+      </c>
+      <c r="H301">
+        <v>12213</v>
+      </c>
+      <c r="I301">
+        <v>0</v>
+      </c>
+      <c r="J301" t="s">
+        <v>37</v>
+      </c>
+      <c r="K301" t="s">
+        <v>37</v>
+      </c>
+      <c r="L301" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="302" spans="1:12">
+      <c r="A302" t="s">
+        <v>258</v>
+      </c>
+      <c r="B302">
+        <v>23</v>
+      </c>
+      <c r="C302">
+        <v>1313043</v>
+      </c>
+      <c r="D302">
+        <v>887742</v>
+      </c>
+      <c r="E302">
+        <v>4371246</v>
+      </c>
+      <c r="F302">
+        <v>121</v>
+      </c>
+      <c r="G302" t="s">
+        <v>21</v>
+      </c>
+      <c r="H302">
+        <v>15632</v>
+      </c>
+      <c r="I302">
+        <v>0</v>
+      </c>
+      <c r="J302" t="s">
+        <v>40</v>
+      </c>
+      <c r="K302" t="s">
+        <v>191</v>
+      </c>
+      <c r="L302" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="303" spans="1:12">
+      <c r="A303" t="s">
+        <v>258</v>
+      </c>
+      <c r="B303">
+        <v>23</v>
+      </c>
+      <c r="C303">
+        <v>1313043</v>
+      </c>
+      <c r="D303">
+        <v>887742</v>
+      </c>
+      <c r="E303">
+        <v>4371246</v>
+      </c>
+      <c r="F303">
+        <v>121</v>
+      </c>
+      <c r="G303" t="s">
+        <v>30</v>
+      </c>
+      <c r="H303">
+        <v>6570</v>
+      </c>
+      <c r="I303">
+        <v>0</v>
+      </c>
+      <c r="J303" t="s">
+        <v>30</v>
+      </c>
+      <c r="K303" t="s">
+        <v>60</v>
+      </c>
+      <c r="L303" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="304" spans="1:12">
+      <c r="A304" t="s">
+        <v>258</v>
+      </c>
+      <c r="B304">
+        <v>23</v>
+      </c>
+      <c r="C304">
+        <v>1313043</v>
+      </c>
+      <c r="D304">
+        <v>887742</v>
+      </c>
+      <c r="E304">
+        <v>4371246</v>
+      </c>
+      <c r="F304">
+        <v>121</v>
+      </c>
+      <c r="G304" t="s">
+        <v>19</v>
+      </c>
+      <c r="H304">
+        <v>24763</v>
+      </c>
+      <c r="I304">
+        <v>0</v>
+      </c>
+      <c r="J304" t="s">
+        <v>38</v>
+      </c>
+      <c r="K304" t="s">
+        <v>52</v>
+      </c>
+      <c r="L304" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="305" spans="1:12">
+      <c r="A305" t="s">
+        <v>258</v>
+      </c>
+      <c r="B305">
+        <v>23</v>
+      </c>
+      <c r="C305">
+        <v>1313043</v>
+      </c>
+      <c r="D305">
+        <v>887742</v>
+      </c>
+      <c r="E305">
+        <v>4371246</v>
+      </c>
+      <c r="F305">
+        <v>121</v>
+      </c>
+      <c r="G305" t="s">
+        <v>227</v>
+      </c>
+      <c r="H305">
+        <v>2941</v>
+      </c>
+      <c r="I305">
+        <v>0</v>
+      </c>
+      <c r="J305" t="s">
+        <v>228</v>
+      </c>
+      <c r="K305" t="s">
+        <v>228</v>
+      </c>
+      <c r="L305" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="306" spans="1:12">
+      <c r="A306" t="s">
+        <v>258</v>
+      </c>
+      <c r="B306">
+        <v>23</v>
+      </c>
+      <c r="C306">
+        <v>1313043</v>
+      </c>
+      <c r="D306">
+        <v>887742</v>
+      </c>
+      <c r="E306">
+        <v>4371246</v>
+      </c>
+      <c r="F306">
+        <v>121</v>
+      </c>
+      <c r="G306" t="s">
+        <v>229</v>
+      </c>
+      <c r="H306">
+        <v>77110</v>
+      </c>
+      <c r="I306">
+        <v>0</v>
+      </c>
+      <c r="J306" t="s">
+        <v>229</v>
+      </c>
+      <c r="K306" t="s">
+        <v>255</v>
+      </c>
+      <c r="L306" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="307" spans="1:12">
+      <c r="A307" t="s">
+        <v>258</v>
+      </c>
+      <c r="B307">
+        <v>23</v>
+      </c>
+      <c r="C307">
+        <v>1313043</v>
+      </c>
+      <c r="D307">
+        <v>887742</v>
+      </c>
+      <c r="E307">
+        <v>4371246</v>
+      </c>
+      <c r="F307">
+        <v>121</v>
+      </c>
+      <c r="G307" t="s">
+        <v>262</v>
+      </c>
+      <c r="H307">
+        <v>1680</v>
+      </c>
+      <c r="I307">
+        <v>0</v>
+      </c>
+      <c r="J307" t="s">
+        <v>26</v>
+      </c>
+      <c r="K307" t="s">
+        <v>267</v>
+      </c>
+      <c r="L307" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>